<commit_message>
Add a lot more quests, mainly complete Rotarycraft chapter (40 quests)
</commit_message>
<xml_diff>
--- a/config/mod-director/bundle.json v5.xlsx
+++ b/config/mod-director/bundle.json v5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason\AppData\Roaming\PrismLauncher\instances\Volentus FileDirector\minecraft\config\mod-director\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCB84FF2-2C9E-47F8-B6E6-2414DBDADBE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E84F4EB-349A-4250-A649-09CFE0A14EE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="839" activeTab="3" xr2:uid="{9C62C9EC-1015-4AFA-B33E-B214A55E5F8C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="839" xr2:uid="{9C62C9EC-1015-4AFA-B33E-B214A55E5F8C}"/>
   </bookViews>
   <sheets>
     <sheet name="CurseForge" sheetId="1" r:id="rId1"/>
@@ -2755,7 +2755,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2774,9 +2774,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -2784,12 +2782,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="23">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2903,6 +2895,9 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor theme="0" tint="-0.14999847407452621"/>
@@ -2945,6 +2940,9 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -3045,7 +3043,7 @@
     <tableColumn id="11" xr3:uid="{D819B850-F57B-498C-825C-8A486975641F}" name="Notes"/>
     <tableColumn id="12" xr3:uid="{49D1682B-534D-4059-A5DA-B3CA78E5F4FB}" name="folder"/>
     <tableColumn id="13" xr3:uid="{4E3663E0-B283-45F0-9C3F-F05498D5CFFD}" name="Repo" dataCellStyle="Hyperlink"/>
-    <tableColumn id="14" xr3:uid="{D8C83F8D-C674-4041-9191-44B2463F4BF7}" name="sourceFileName" dataDxfId="1">
+    <tableColumn id="14" xr3:uid="{D8C83F8D-C674-4041-9191-44B2463F4BF7}" name="sourceFileName" dataDxfId="20">
       <calculatedColumnFormula>IF(H2&lt;&gt;"", H2, RIGHT(F2,LEN(F2)-FIND("@",SUBSTITUTE(F2,"/","@",LEN(F2)-LEN(SUBSTITUTE(F2,"/",""))))))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="15" xr3:uid="{AC8070E0-756B-431E-A1EC-4CB67F73C9E2}" name="followsIL"/>
@@ -3055,7 +3053,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{837A1DAE-8158-4E48-816C-7B02D8E95473}" name="Table6" displayName="Table6" ref="A1:M28" totalsRowShown="0" headerRowDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{837A1DAE-8158-4E48-816C-7B02D8E95473}" name="Table6" displayName="Table6" ref="A1:M28" totalsRowShown="0" headerRowDxfId="19">
   <autoFilter ref="A1:M28" xr:uid="{837A1DAE-8158-4E48-816C-7B02D8E95473}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L28">
     <sortCondition ref="E1:E28"/>
@@ -3084,17 +3082,17 @@
   <autoFilter ref="E1:N13" xr:uid="{8FA21BC5-EE0E-4191-BC63-9EB4198DCDF8}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{60D5533B-280C-4133-820D-E94C6E9E36DB}" name="name"/>
-    <tableColumn id="2" xr3:uid="{66EF7A2B-9A21-4085-93F7-14CD58F6F15B}" name="url" dataDxfId="19" dataCellStyle="Hyperlink"/>
+    <tableColumn id="2" xr3:uid="{66EF7A2B-9A21-4085-93F7-14CD58F6F15B}" name="url" dataDxfId="18" dataCellStyle="Hyperlink"/>
     <tableColumn id="3" xr3:uid="{C0731F1D-4A65-4CA3-9F35-0689AF888300}" name="side"/>
     <tableColumn id="4" xr3:uid="{20970281-086F-4DD1-BF01-7E06711A2DDF}" name="fileName"/>
     <tableColumn id="5" xr3:uid="{B177552A-E452-47D5-80D6-29CB46C2F510}" name="follows"/>
     <tableColumn id="6" xr3:uid="{1962D553-6A3F-4CA6-927C-7A94E4C9757F}" name="License"/>
     <tableColumn id="7" xr3:uid="{48F547D9-B9D6-48B9-BAA7-B1972742C050}" name="Notes"/>
     <tableColumn id="8" xr3:uid="{948716AE-E46C-40AC-A5A6-5231FDD8884A}" name="folder"/>
-    <tableColumn id="9" xr3:uid="{4F45D914-640E-4DCB-A55E-32DFDD6BE6BC}" name="Repo" dataDxfId="18" dataCellStyle="Hyperlink">
+    <tableColumn id="9" xr3:uid="{4F45D914-640E-4DCB-A55E-32DFDD6BE6BC}" name="Repo" dataDxfId="17" dataCellStyle="Hyperlink">
       <calculatedColumnFormula>LEFT(F2, FIND("/releases", F2) - 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{82D64721-6A58-4E8F-B4CC-4E9A79C19880}" name="sourceFileName" dataDxfId="0">
+    <tableColumn id="10" xr3:uid="{82D64721-6A58-4E8F-B4CC-4E9A79C19880}" name="sourceFileName" dataDxfId="16">
       <calculatedColumnFormula>IF(H2&lt;&gt;"", H2, RIGHT(F2,LEN(F2)-FIND("@",SUBSTITUTE(F2,"/","@",LEN(F2)-LEN(SUBSTITUTE(F2,"/",""))))))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3404,12 +3402,12 @@
   </sheetPr>
   <dimension ref="A1:M155"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="F135" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
-      <selection pane="bottomRight" activeCell="S149" sqref="S149"/>
+      <selection pane="bottomRight" activeCell="K153" sqref="K153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -6388,18 +6386,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I1:J98 I156:J1048576">
-    <cfRule type="cellIs" dxfId="17" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="7" operator="equal">
       <formula>"Custom License"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="8" operator="equal">
       <formula>"All Rights Reserved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I101:J155">
-    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
       <formula>"Custom License"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
       <formula>"All Rights Reserved"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6484,19 +6482,13 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="16" t="s">
+      <c r="A6" t="s">
         <v>441</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="16" t="s">
         <v>442</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="17" t="str">
+      <c r="I6" s="16" t="str">
         <f>LEFT(B6, FIND("/releases", B6) - 1)</f>
         <v>https://github.com/age-series/ElectricalAge</v>
       </c>
@@ -6518,9 +6510,9 @@
   <dimension ref="A1:O119"/>
   <sheetViews>
     <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="E33" sqref="E33"/>
+      <selection pane="bottomLeft" activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -7654,7 +7646,7 @@
         <v>276</v>
       </c>
       <c r="M62" s="4" t="e">
-        <f>LEFT(F62, FIND("/releases", F62) - 1)</f>
+        <f t="shared" ref="M62:M93" si="4">LEFT(F62, FIND("/releases", F62) - 1)</f>
         <v>#VALUE!</v>
       </c>
       <c r="N62" t="str">
@@ -7673,7 +7665,7 @@
         <v>302</v>
       </c>
       <c r="M63" s="4" t="str">
-        <f>LEFT(F63, FIND("/releases", F63) - 1)</f>
+        <f t="shared" si="4"/>
         <v>https://github.com/Jonius7/FullThrottleAlchemistFix</v>
       </c>
       <c r="N63" t="str">
@@ -7692,7 +7684,7 @@
         <v>363</v>
       </c>
       <c r="M64" s="4" t="e">
-        <f>LEFT(F64, FIND("/releases", F64) - 1)</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="N64" t="str">
@@ -7708,7 +7700,7 @@
         <v>349</v>
       </c>
       <c r="M65" s="4" t="str">
-        <f>LEFT(F65, FIND("/releases", F65) - 1)</f>
+        <f t="shared" si="4"/>
         <v>https://github.com/GTNewHorizons/EnderIO</v>
       </c>
       <c r="N65" t="str">
@@ -7724,11 +7716,11 @@
         <v>352</v>
       </c>
       <c r="M66" s="4" t="e">
-        <f>LEFT(F66, FIND("/releases", F66) - 1)</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="N66" t="str">
-        <f t="shared" ref="N66:N97" si="4">IF(H66&lt;&gt;"", H66, RIGHT(F66,LEN(F66)-FIND("@",SUBSTITUTE(F66,"/","@",LEN(F66)-LEN(SUBSTITUTE(F66,"/",""))))))</f>
+        <f t="shared" ref="N66:N97" si="5">IF(H66&lt;&gt;"", H66, RIGHT(F66,LEN(F66)-FIND("@",SUBSTITUTE(F66,"/","@",LEN(F66)-LEN(SUBSTITUTE(F66,"/",""))))))</f>
         <v>TooManyDanyOres-1.7.10-b1.0-3-forge-1199.jar</v>
       </c>
     </row>
@@ -7743,11 +7735,11 @@
         <v>276</v>
       </c>
       <c r="M67" s="4" t="e">
-        <f>LEFT(F67, FIND("/releases", F67) - 1)</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="N67" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>advancedgenetics-1.7.10-1.5.9.jar</v>
       </c>
     </row>
@@ -7762,11 +7754,11 @@
         <v>276</v>
       </c>
       <c r="M68" s="4" t="e">
-        <f>LEFT(F68, FIND("/releases", F68) - 1)</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="N68" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>adv-repulsion-systems-59.0.4.jar</v>
       </c>
     </row>
@@ -7781,11 +7773,11 @@
         <v>366</v>
       </c>
       <c r="M69" s="4" t="e">
-        <f>LEFT(F69, FIND("/releases", F69) - 1)</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="N69" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>AdvancedSolarPanel-1.7.10-3.5.1.jar</v>
       </c>
     </row>
@@ -7797,11 +7789,11 @@
         <v>368</v>
       </c>
       <c r="M70" s="4" t="str">
-        <f>LEFT(F70, FIND("/releases", F70) - 1)</f>
+        <f t="shared" si="4"/>
         <v>https://github.com/GTNewHorizons/ae2stuff</v>
       </c>
       <c r="N70" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>ae2stuff-0.9.7-GTNH.jar</v>
       </c>
     </row>
@@ -7813,11 +7805,11 @@
         <v>375</v>
       </c>
       <c r="M71" s="4" t="e">
-        <f>LEFT(F71, FIND("/releases", F71) - 1)</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="N71" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>AOBD-2.9.2.jar</v>
       </c>
     </row>
@@ -7829,11 +7821,11 @@
         <v>376</v>
       </c>
       <c r="M72" s="4" t="e">
-        <f>LEFT(F72, FIND("/releases", F72) - 1)</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="N72" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>AOBDBB-1.0.6.jar</v>
       </c>
     </row>
@@ -7851,11 +7843,11 @@
         <v>277</v>
       </c>
       <c r="M73" s="4" t="str">
-        <f>LEFT(F73, FIND("/releases", F73) - 1)</f>
+        <f t="shared" si="4"/>
         <v>https://github.com/GTNewHorizons/AntiqueAtlas</v>
       </c>
       <c r="N73" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>antiqueatlas-4.4.6-GTNH.jar</v>
       </c>
     </row>
@@ -7867,11 +7859,11 @@
         <v>379</v>
       </c>
       <c r="M74" s="4" t="str">
-        <f>LEFT(F74, FIND("/releases", F74) - 1)</f>
+        <f t="shared" si="4"/>
         <v>https://github.com/GTNewHorizons/WirelessCraftingTerminal</v>
       </c>
       <c r="N74" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>WirelessCraftingTerminal-1.12.7.jar</v>
       </c>
     </row>
@@ -7886,11 +7878,11 @@
         <v>283</v>
       </c>
       <c r="M75" s="4" t="str">
-        <f>LEFT(F75, FIND("/releases", F75) - 1)</f>
+        <f t="shared" si="4"/>
         <v>https://github.com/GTNewHorizons/ArchitectureCraft</v>
       </c>
       <c r="N75" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>ArchitectureCraft-1.11.4.jar</v>
       </c>
     </row>
@@ -7905,11 +7897,11 @@
         <v>283</v>
       </c>
       <c r="M76" s="4" t="str">
-        <f>LEFT(F76, FIND("/releases", F76) - 1)</f>
+        <f t="shared" si="4"/>
         <v>https://github.com/GTNewHorizons/Computronics</v>
       </c>
       <c r="N76" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Computronics-1.9.3-GTNH.jar</v>
       </c>
     </row>
@@ -7924,11 +7916,11 @@
         <v>302</v>
       </c>
       <c r="M77" s="4" t="str">
-        <f>LEFT(F77, FIND("/releases", F77) - 1)</f>
+        <f t="shared" si="4"/>
         <v>https://github.com/GTNewHorizons/Minecraft-Backpack-Mod</v>
       </c>
       <c r="N77" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>backpack-2.5.6-GTNH.jar</v>
       </c>
     </row>
@@ -7943,11 +7935,11 @@
         <v>283</v>
       </c>
       <c r="M78" s="4" t="str">
-        <f>LEFT(F78, FIND("/releases", F78) - 1)</f>
+        <f t="shared" si="4"/>
         <v>https://github.com/copygirl/BetterStorage</v>
       </c>
       <c r="N78" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>BetterStorage-1.7.10-0.13.1.128.jar</v>
       </c>
     </row>
@@ -7959,11 +7951,11 @@
         <v>408</v>
       </c>
       <c r="M79" s="4" t="str">
-        <f>LEFT(F79, FIND("/releases", F79) - 1)</f>
+        <f t="shared" si="4"/>
         <v>https://github.com/GTNewHorizons/BeeBetterAtBees-GTNH</v>
       </c>
       <c r="N79" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>beebetteratbees-0.4.3-GTNH.jar</v>
       </c>
     </row>
@@ -7978,11 +7970,11 @@
         <v>426</v>
       </c>
       <c r="M80" s="4" t="str">
-        <f>LEFT(F80, FIND("/releases", F80) - 1)</f>
+        <f t="shared" si="4"/>
         <v>https://github.com/GTNewHorizons/CarpentersBlocks</v>
       </c>
       <c r="N80" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>CarpentersBlocks-3.7.0-GTNH.jar</v>
       </c>
     </row>
@@ -7997,11 +7989,11 @@
         <v>431</v>
       </c>
       <c r="M81" s="4" t="str">
-        <f>LEFT(F81, FIND("/releases", F81) - 1)</f>
+        <f t="shared" si="4"/>
         <v>https://github.com/GTNewHorizons/CookingForBlockheads</v>
       </c>
       <c r="N81" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>CookingForBlockheads-1.4.4-GTNH.jar</v>
       </c>
     </row>
@@ -8013,11 +8005,11 @@
         <v>435</v>
       </c>
       <c r="M82" s="4" t="str">
-        <f>LEFT(F82, FIND("/releases", F82) - 1)</f>
+        <f t="shared" si="4"/>
         <v>https://github.com/GTNewHorizons/CraftingTweaks</v>
       </c>
       <c r="N82" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>craftingtweaks-1.1.0-GTNH.jar</v>
       </c>
     </row>
@@ -8029,11 +8021,11 @@
         <v>438</v>
       </c>
       <c r="M83" s="4" t="e">
-        <f>LEFT(F83, FIND("/releases", F83) - 1)</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="N83" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>cogs-1.7.10-0.1.4.jar</v>
       </c>
     </row>
@@ -8045,11 +8037,11 @@
         <v>178</v>
       </c>
       <c r="M84" s="4" t="str">
-        <f>LEFT(F84, FIND("/releases", F84) - 1)</f>
+        <f t="shared" si="4"/>
         <v>https://github.com/GTNewHorizons/Draconic-Evolution</v>
       </c>
       <c r="N84" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Draconic-Evolution-1.4.24-GTNH.jar</v>
       </c>
     </row>
@@ -8064,11 +8056,11 @@
         <v>255</v>
       </c>
       <c r="M85" s="4" t="str">
-        <f>LEFT(F85, FIND("/releases", F85) - 1)</f>
+        <f t="shared" si="4"/>
         <v>https://github.com/Jonius7/ElectricalAge</v>
       </c>
       <c r="N85" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Eln-1.22.4.jar</v>
       </c>
     </row>
@@ -8083,11 +8075,11 @@
         <v>283</v>
       </c>
       <c r="M86" s="4" t="str">
-        <f>LEFT(F86, FIND("/releases", F86) - 1)</f>
+        <f t="shared" si="4"/>
         <v>https://github.com/GTNewHorizons/EnderStorage</v>
       </c>
       <c r="N86" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>EnderStorage-1.7.7.jar</v>
       </c>
     </row>
@@ -8102,11 +8094,11 @@
         <v>283</v>
       </c>
       <c r="M87" s="4" t="str">
-        <f>LEFT(F87, FIND("/releases", F87) - 1)</f>
+        <f t="shared" si="4"/>
         <v>https://github.com/GTNewHorizons/ExtraCells2</v>
       </c>
       <c r="N87" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>ExtraCells-2.5.35.jar</v>
       </c>
     </row>
@@ -8118,11 +8110,11 @@
         <v>460</v>
       </c>
       <c r="M88" s="4" t="str">
-        <f>LEFT(F88, FIND("/releases", F88) - 1)</f>
+        <f t="shared" si="4"/>
         <v>https://github.com/GTNewHorizons/ForbiddenMagic</v>
       </c>
       <c r="N88" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>Forbidden.Magic-0.8.3-GTNH.jar</v>
       </c>
     </row>
@@ -8134,11 +8126,11 @@
         <v>462</v>
       </c>
       <c r="M89" s="4" t="str">
-        <f>LEFT(F89, FIND("/releases", F89) - 1)</f>
+        <f t="shared" si="4"/>
         <v>https://github.com/GTNewHorizons/ForgeRelocationFMP</v>
       </c>
       <c r="N89" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>ForgeRelocationFMP-0.2.0.jar</v>
       </c>
     </row>
@@ -8153,11 +8145,11 @@
         <v>302</v>
       </c>
       <c r="M90" s="4" t="str">
-        <f>LEFT(F90, FIND("/releases", F90) - 1)</f>
+        <f t="shared" si="4"/>
         <v>https://github.com/GTNewHorizons/Gadomancy</v>
       </c>
       <c r="N90" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>gadomancy-1.4.7.jar</v>
       </c>
     </row>
@@ -8169,11 +8161,11 @@
         <v>474</v>
       </c>
       <c r="M91" s="4" t="e">
-        <f>LEFT(F91, FIND("/releases", F91) - 1)</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="N91" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>immibis-macroblocks-59.1.1.jar</v>
       </c>
     </row>
@@ -8185,11 +8177,11 @@
         <v>476</v>
       </c>
       <c r="M92" s="4" t="e">
-        <f>LEFT(F92, FIND("/releases", F92) - 1)</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="N92" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>immibis-peripherals-59.0.3.jar</v>
       </c>
     </row>
@@ -8201,11 +8193,11 @@
         <v>478</v>
       </c>
       <c r="M93" s="4" t="e">
-        <f>LEFT(F93, FIND("/releases", F93) - 1)</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="N93" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>infinitubes-59.0.5.jar</v>
       </c>
     </row>
@@ -8217,11 +8209,11 @@
         <v>480</v>
       </c>
       <c r="M94" s="4" t="e">
-        <f t="shared" ref="M94:M118" si="5">LEFT(F94, FIND("/releases", F94) - 1)</f>
+        <f t="shared" ref="M94:M118" si="6">LEFT(F94, FIND("/releases", F94) - 1)</f>
         <v>#VALUE!</v>
       </c>
       <c r="N94" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>liquid-xp-59.0.2.jar</v>
       </c>
     </row>
@@ -8236,11 +8228,11 @@
         <v>250</v>
       </c>
       <c r="M95" s="4" t="e">
+        <f t="shared" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N95" t="str">
         <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N95" t="str">
-        <f t="shared" si="4"/>
         <v>IGW-Mod-1.7.10-1.1.12-34-universal.jar</v>
       </c>
     </row>
@@ -8255,11 +8247,11 @@
         <v>488</v>
       </c>
       <c r="M96" s="4" t="str">
+        <f t="shared" si="6"/>
+        <v>https://github.com/GTNewHorizons/LogisticsPipes</v>
+      </c>
+      <c r="N96" t="str">
         <f t="shared" si="5"/>
-        <v>https://github.com/GTNewHorizons/LogisticsPipes</v>
-      </c>
-      <c r="N96" t="str">
-        <f t="shared" si="4"/>
         <v>logisticspipes-1.4.23-GTNH-pre.jar</v>
       </c>
     </row>
@@ -8271,11 +8263,11 @@
         <v>508</v>
       </c>
       <c r="M97" s="4" t="e">
+        <f t="shared" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N97" t="str">
         <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N97" t="str">
-        <f t="shared" si="4"/>
         <v>PneumaticCompressing-1.0.5.jar</v>
       </c>
     </row>
@@ -8287,11 +8279,11 @@
         <v>210</v>
       </c>
       <c r="M98" s="4" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="N98" t="str">
-        <f t="shared" ref="N98:N119" si="6">IF(H98&lt;&gt;"", H98, RIGHT(F98,LEN(F98)-FIND("@",SUBSTITUTE(F98,"/","@",LEN(F98)-LEN(SUBSTITUTE(F98,"/",""))))))</f>
+        <f t="shared" ref="N98:N119" si="7">IF(H98&lt;&gt;"", H98, RIGHT(F98,LEN(F98)-FIND("@",SUBSTITUTE(F98,"/","@",LEN(F98)-LEN(SUBSTITUTE(F98,"/",""))))))</f>
         <v>SolarExpansion-Basic-1.6a.jar</v>
       </c>
     </row>
@@ -8306,11 +8298,11 @@
         <v>277</v>
       </c>
       <c r="M99" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>https://github.com/GTNewHorizons/ThaumicEnergistics</v>
       </c>
       <c r="N99" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>thaumicenergistics-1.7.11-GTNH.jar</v>
       </c>
     </row>
@@ -8325,11 +8317,11 @@
         <v>516</v>
       </c>
       <c r="M100" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>https://github.com/GTNewHorizons/Thaumic_Exploration</v>
       </c>
       <c r="N100" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>Thaumic-Exploration-1.4.6-GTNH-pre.jar</v>
       </c>
     </row>
@@ -8344,11 +8336,11 @@
         <v>523</v>
       </c>
       <c r="M101" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>https://github.com/GTNewHorizons/ThaumicTinkerer</v>
       </c>
       <c r="N101" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>ThaumicTinkerer-2.11.20.jar</v>
       </c>
     </row>
@@ -8363,11 +8355,11 @@
         <v>426</v>
       </c>
       <c r="M102" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>https://github.com/GTNewHorizons/twilightforest</v>
       </c>
       <c r="N102" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>TwilightForest-2.7.11.jar</v>
       </c>
     </row>
@@ -8385,11 +8377,11 @@
         <v>531</v>
       </c>
       <c r="M103" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>https://github.com/GTNewHorizons/TiC-Tooltips</v>
       </c>
       <c r="N103" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>TiCTooltips-1.4.0.jar</v>
       </c>
     </row>
@@ -8404,11 +8396,11 @@
         <v>283</v>
       </c>
       <c r="M104" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>https://github.com/GTNewHorizons/TinkersMechworks</v>
       </c>
       <c r="N104" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>TMechworks-0.4.1.jar</v>
       </c>
     </row>
@@ -8420,11 +8412,11 @@
         <v>540</v>
       </c>
       <c r="M105" s="4" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="N105" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>tubestuff-59.0.4.jar</v>
       </c>
     </row>
@@ -8436,11 +8428,11 @@
         <v>544</v>
       </c>
       <c r="M106" s="4" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="N106" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>UniverseCraft-1.7.10-V1.4.2.jar</v>
       </c>
     </row>
@@ -8452,11 +8444,11 @@
         <v>553</v>
       </c>
       <c r="M107" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>https://github.com/GTNewHorizons/gendustry</v>
       </c>
       <c r="N107" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>gendustry-1.9.4-GTNH.jar</v>
       </c>
     </row>
@@ -8468,11 +8460,11 @@
         <v>559</v>
       </c>
       <c r="M108" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>https://github.com/Jonius7/EnderIOAddons</v>
       </c>
       <c r="N108" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>enderioaddons-1.7.10-0.10.16.jar</v>
       </c>
     </row>
@@ -8490,11 +8482,11 @@
         <v>563</v>
       </c>
       <c r="M109" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>https://github.com/GTNewHorizons/AkashicTome</v>
       </c>
       <c r="N109" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>akashictome-1.2.6.jar</v>
       </c>
     </row>
@@ -8512,11 +8504,11 @@
         <v>283</v>
       </c>
       <c r="M110" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>https://github.com/idkidknow/IE1710NEIPatch</v>
       </c>
       <c r="N110" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>ie1710neipatch-0.1.1.jar</v>
       </c>
     </row>
@@ -8528,11 +8520,11 @@
         <v>572</v>
       </c>
       <c r="M111" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>https://github.com/GTNewHorizons/FTB-Utilities</v>
       </c>
       <c r="N111" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>FTBUtilities-1.1.1-GTNH.jar</v>
       </c>
     </row>
@@ -8544,11 +8536,11 @@
         <v>577</v>
       </c>
       <c r="M112" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>https://github.com/GTNewHorizons/Nuclear-Control</v>
       </c>
       <c r="N112" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>IC2NuclearControl-2.6.19.jar</v>
       </c>
     </row>
@@ -8563,11 +8555,11 @@
         <v>254</v>
       </c>
       <c r="M113" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>https://github.com/GTNewHorizons/ProjectBlue</v>
       </c>
       <c r="N113" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>ProjectBlue-1.2.0-GTNH.jar</v>
       </c>
     </row>
@@ -8582,11 +8574,11 @@
         <v>283</v>
       </c>
       <c r="M114" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>https://github.com/GTNewHorizons/WirelessRedstone-CBE</v>
       </c>
       <c r="N114" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>WR-CBE-1.7.1.jar</v>
       </c>
     </row>
@@ -8601,11 +8593,11 @@
         <v>297</v>
       </c>
       <c r="M115" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>https://github.com/GTNewHorizons/Chisel</v>
       </c>
       <c r="N115" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>chisel-2.16.11-GTNH.jar</v>
       </c>
     </row>
@@ -8620,11 +8612,11 @@
         <v>591</v>
       </c>
       <c r="M116" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>https://github.com/DrParadox7/Binnie</v>
       </c>
       <c r="N116" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>binnie-mods-v2.1.15-LE.jar</v>
       </c>
     </row>
@@ -8639,11 +8631,11 @@
         <v>283</v>
       </c>
       <c r="M117" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>https://github.com/Jonius7/NuclearCraft</v>
       </c>
       <c r="N117" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>NuclearCraft-1.9h--1.7.10.jar</v>
       </c>
     </row>
@@ -8658,11 +8650,11 @@
         <v>283</v>
       </c>
       <c r="M118" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>https://github.com/GTNewHorizons/BetterQuesting</v>
       </c>
       <c r="N118" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>BetterQuesting-3.7.13-GTNH.jar</v>
       </c>
     </row>
@@ -8670,23 +8662,23 @@
       <c r="E119" t="s">
         <v>684</v>
       </c>
-      <c r="F119" s="18" t="s">
+      <c r="F119" s="4" t="s">
         <v>685</v>
       </c>
       <c r="H119" t="s">
         <v>686</v>
       </c>
       <c r="N119" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>ztech1.7.10-0.0.3.jar</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="J3">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>"Custom License"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
       <formula>"All Rights Reserved"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8821,12 +8813,12 @@
   </sheetPr>
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F14" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="F11" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
-      <selection pane="bottomRight" activeCell="L26" sqref="L26"/>
+      <selection pane="bottomRight" activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -9428,10 +9420,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I1:I28 I30:I1048576">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>"Custom License"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
       <formula>"All Rights Reserved"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9519,7 +9511,7 @@
       <c r="F2" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="M2" s="19" t="str">
+      <c r="M2" s="17" t="str">
         <f t="shared" ref="M2:M12" si="0">LEFT(F2, FIND("/releases", F2) - 1)</f>
         <v>https://github.com/Jonius7/Mantle</v>
       </c>
@@ -9535,7 +9527,7 @@
       <c r="F3" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="M3" s="19" t="str">
+      <c r="M3" s="17" t="str">
         <f t="shared" si="0"/>
         <v>https://github.com/GTNewHorizons/EnderCore</v>
       </c>
@@ -9551,7 +9543,7 @@
       <c r="F4" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="M4" s="19" t="str">
+      <c r="M4" s="17" t="str">
         <f t="shared" si="0"/>
         <v>https://github.com/GTNewHorizons/OpenModsLib</v>
       </c>
@@ -9567,7 +9559,7 @@
       <c r="F5" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="M5" s="19" t="str">
+      <c r="M5" s="17" t="str">
         <f t="shared" si="0"/>
         <v>https://github.com/GTNewHorizons/MrTJPCore</v>
       </c>
@@ -9583,7 +9575,7 @@
       <c r="F6" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="M6" s="19" t="str">
+      <c r="M6" s="17" t="str">
         <f t="shared" si="0"/>
         <v>https://github.com/GTNewHorizons/BrandonsCore</v>
       </c>
@@ -9599,7 +9591,7 @@
       <c r="F7" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="M7" s="19" t="str">
+      <c r="M7" s="17" t="str">
         <f t="shared" si="0"/>
         <v>https://github.com/GTNewHorizons/LunatriusCore</v>
       </c>
@@ -9615,7 +9607,7 @@
       <c r="F8" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="M8" s="19" t="e">
+      <c r="M8" s="17" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
@@ -9634,7 +9626,7 @@
       <c r="J9" t="s">
         <v>257</v>
       </c>
-      <c r="M9" s="19" t="str">
+      <c r="M9" s="17" t="str">
         <f t="shared" si="0"/>
         <v>https://github.com/GTNewHorizons/AsieLib</v>
       </c>
@@ -9653,7 +9645,7 @@
       <c r="J10" t="s">
         <v>417</v>
       </c>
-      <c r="M10" s="19" t="str">
+      <c r="M10" s="17" t="str">
         <f t="shared" si="0"/>
         <v>https://github.com/GTNewHorizons/bdlib</v>
       </c>
@@ -9669,7 +9661,7 @@
       <c r="F11" s="4" t="s">
         <v>557</v>
       </c>
-      <c r="M11" s="19" t="str">
+      <c r="M11" s="17" t="str">
         <f t="shared" si="0"/>
         <v>https://github.com/GTNewHorizons/ModularUI2</v>
       </c>
@@ -9685,7 +9677,7 @@
       <c r="F12" s="4" t="s">
         <v>573</v>
       </c>
-      <c r="M12" s="19" t="str">
+      <c r="M12" s="17" t="str">
         <f t="shared" si="0"/>
         <v>https://github.com/GTNewHorizons/FTB-Library</v>
       </c>
@@ -9711,7 +9703,7 @@
       <c r="L13" s="9" t="s">
         <v>289</v>
       </c>
-      <c r="M13" s="19" t="str">
+      <c r="M13" s="17" t="str">
         <f>LEFT(F13, FIND("/releases", F13) - 1)</f>
         <v>https://github.com/GTNewHorizons/ForgeMultipart</v>
       </c>
@@ -9913,7 +9905,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10432,34 +10424,34 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E6:E18">
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>"Custom License"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
       <formula>"All Rights Reserved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20:E22">
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>"Custom License"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"All Rights Reserved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19:F19">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>"Custom License"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
       <formula>"All Rights Reserved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23:F23">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Custom License"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"All Rights Reserved"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Fleshed out Inductive Automation Quests, Started Ender IO
</commit_message>
<xml_diff>
--- a/config/mod-director/bundle.json v5.xlsx
+++ b/config/mod-director/bundle.json v5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason\AppData\Roaming\PrismLauncher\instances\Volentus FileDirector\minecraft\config\mod-director\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E84F4EB-349A-4250-A649-09CFE0A14EE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5D7BB87-83D6-4669-BD01-B660288B8746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="839" xr2:uid="{9C62C9EC-1015-4AFA-B33E-B214A55E5F8C}"/>
+    <workbookView xWindow="300" yWindow="132" windowWidth="22392" windowHeight="12024" tabRatio="839" xr2:uid="{9C62C9EC-1015-4AFA-B33E-B214A55E5F8C}"/>
   </bookViews>
   <sheets>
     <sheet name="CurseForge" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Fleshed out Botania and Thermal Expansion quests
</commit_message>
<xml_diff>
--- a/config/mod-director/bundle.json v5.xlsx
+++ b/config/mod-director/bundle.json v5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason\AppData\Roaming\PrismLauncher\instances\Volentus FileDirector\minecraft\config\mod-director\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5D7BB87-83D6-4669-BD01-B660288B8746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92710FFA-F579-43CE-B8D0-4FAD65564543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="132" windowWidth="22392" windowHeight="12024" tabRatio="839" xr2:uid="{9C62C9EC-1015-4AFA-B33E-B214A55E5F8C}"/>
+    <workbookView xWindow="1332" yWindow="216" windowWidth="22392" windowHeight="12024" tabRatio="839" activeTab="3" xr2:uid="{9C62C9EC-1015-4AFA-B33E-B214A55E5F8C}"/>
   </bookViews>
   <sheets>
     <sheet name="CurseForge" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1192" uniqueCount="872">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1202" uniqueCount="880">
   <si>
     <t>addonId</t>
   </si>
@@ -2659,6 +2659,30 @@
   </si>
   <si>
     <t>https://www.curseforge.com/minecraft/mc-mods/wanionlib</t>
+  </si>
+  <si>
+    <t>Technomancy - 0.12.5 - 1.7.10.jar</t>
+  </si>
+  <si>
+    <t>Technomancy</t>
+  </si>
+  <si>
+    <t>https://mediafilez.forgecdn.net/files/2295/819/Technomancy - 0.12.5 - 1.7.10.jar</t>
+  </si>
+  <si>
+    <t>Thaumic Expansion</t>
+  </si>
+  <si>
+    <t>https://www.curseforge.com/minecraft/mc-mods/thaumic-expansion</t>
+  </si>
+  <si>
+    <t>Origin</t>
+  </si>
+  <si>
+    <t>https://www.curseforge.com/minecraft/mc-mods/origin</t>
+  </si>
+  <si>
+    <t>Origin-1.7.10-8.0.3.jar</t>
   </si>
 </sst>
 </file>
@@ -2781,7 +2805,21 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="25">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6565"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2999,8 +3037,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CF71CB59-A681-467E-A496-DF22C8F63C36}" name="Table1" displayName="Table1" ref="A1:M155" totalsRowShown="0" headerRowDxfId="22">
-  <autoFilter ref="A1:M155" xr:uid="{CF71CB59-A681-467E-A496-DF22C8F63C36}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CF71CB59-A681-467E-A496-DF22C8F63C36}" name="Table1" displayName="Table1" ref="A1:M156" totalsRowShown="0" headerRowDxfId="24">
+  <autoFilter ref="A1:M156" xr:uid="{CF71CB59-A681-467E-A496-DF22C8F63C36}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L80">
     <sortCondition ref="E1:E80"/>
   </sortState>
@@ -3024,8 +3062,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8C69A2DD-805E-41CC-A56E-3CB65AD41149}" name="Table2" displayName="Table2" ref="A1:O119" totalsRowShown="0">
-  <autoFilter ref="A1:O119" xr:uid="{8C69A2DD-805E-41CC-A56E-3CB65AD41149}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8C69A2DD-805E-41CC-A56E-3CB65AD41149}" name="Table2" displayName="Table2" ref="A1:O120" totalsRowShown="0">
+  <autoFilter ref="A1:O120" xr:uid="{8C69A2DD-805E-41CC-A56E-3CB65AD41149}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E2:I28">
     <sortCondition ref="E1:E28"/>
   </sortState>
@@ -3035,7 +3073,7 @@
     <tableColumn id="8" xr3:uid="{071FB076-79DA-4271-9B11-D3DAF5A27A08}" name="selectedByDefault"/>
     <tableColumn id="9" xr3:uid="{3CDEFED8-BDC9-47C7-831C-532778102D77}" name="description"/>
     <tableColumn id="1" xr3:uid="{E6FB84AB-CA8F-4CC7-B1A7-BC7A68F80D0F}" name="name"/>
-    <tableColumn id="2" xr3:uid="{F0A7EA2F-C2AC-43F5-BC6D-C49D0647EFC8}" name="url" dataDxfId="21" dataCellStyle="Hyperlink"/>
+    <tableColumn id="2" xr3:uid="{F0A7EA2F-C2AC-43F5-BC6D-C49D0647EFC8}" name="url" dataDxfId="23" dataCellStyle="Hyperlink"/>
     <tableColumn id="6" xr3:uid="{EC64C9C3-AEEF-4EBD-8BFF-4E2922D06865}" name="side"/>
     <tableColumn id="4" xr3:uid="{9F48CDE4-D924-41EA-B9F4-C5D89CD73B03}" name="fileName"/>
     <tableColumn id="5" xr3:uid="{7F05F574-DA53-49C9-8050-3D2CCDAB677A}" name="follows"/>
@@ -3043,7 +3081,7 @@
     <tableColumn id="11" xr3:uid="{D819B850-F57B-498C-825C-8A486975641F}" name="Notes"/>
     <tableColumn id="12" xr3:uid="{49D1682B-534D-4059-A5DA-B3CA78E5F4FB}" name="folder"/>
     <tableColumn id="13" xr3:uid="{4E3663E0-B283-45F0-9C3F-F05498D5CFFD}" name="Repo" dataCellStyle="Hyperlink"/>
-    <tableColumn id="14" xr3:uid="{D8C83F8D-C674-4041-9191-44B2463F4BF7}" name="sourceFileName" dataDxfId="20">
+    <tableColumn id="14" xr3:uid="{D8C83F8D-C674-4041-9191-44B2463F4BF7}" name="sourceFileName" dataDxfId="22">
       <calculatedColumnFormula>IF(H2&lt;&gt;"", H2, RIGHT(F2,LEN(F2)-FIND("@",SUBSTITUTE(F2,"/","@",LEN(F2)-LEN(SUBSTITUTE(F2,"/",""))))))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="15" xr3:uid="{AC8070E0-756B-431E-A1EC-4CB67F73C9E2}" name="followsIL"/>
@@ -3053,8 +3091,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{837A1DAE-8158-4E48-816C-7B02D8E95473}" name="Table6" displayName="Table6" ref="A1:M28" totalsRowShown="0" headerRowDxfId="19">
-  <autoFilter ref="A1:M28" xr:uid="{837A1DAE-8158-4E48-816C-7B02D8E95473}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{837A1DAE-8158-4E48-816C-7B02D8E95473}" name="Table6" displayName="Table6" ref="A1:M29" totalsRowShown="0" headerRowDxfId="21">
+  <autoFilter ref="A1:M29" xr:uid="{837A1DAE-8158-4E48-816C-7B02D8E95473}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L28">
     <sortCondition ref="E1:E28"/>
   </sortState>
@@ -3082,17 +3120,17 @@
   <autoFilter ref="E1:N13" xr:uid="{8FA21BC5-EE0E-4191-BC63-9EB4198DCDF8}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{60D5533B-280C-4133-820D-E94C6E9E36DB}" name="name"/>
-    <tableColumn id="2" xr3:uid="{66EF7A2B-9A21-4085-93F7-14CD58F6F15B}" name="url" dataDxfId="18" dataCellStyle="Hyperlink"/>
+    <tableColumn id="2" xr3:uid="{66EF7A2B-9A21-4085-93F7-14CD58F6F15B}" name="url" dataDxfId="20" dataCellStyle="Hyperlink"/>
     <tableColumn id="3" xr3:uid="{C0731F1D-4A65-4CA3-9F35-0689AF888300}" name="side"/>
     <tableColumn id="4" xr3:uid="{20970281-086F-4DD1-BF01-7E06711A2DDF}" name="fileName"/>
     <tableColumn id="5" xr3:uid="{B177552A-E452-47D5-80D6-29CB46C2F510}" name="follows"/>
     <tableColumn id="6" xr3:uid="{1962D553-6A3F-4CA6-927C-7A94E4C9757F}" name="License"/>
     <tableColumn id="7" xr3:uid="{48F547D9-B9D6-48B9-BAA7-B1972742C050}" name="Notes"/>
     <tableColumn id="8" xr3:uid="{948716AE-E46C-40AC-A5A6-5231FDD8884A}" name="folder"/>
-    <tableColumn id="9" xr3:uid="{4F45D914-640E-4DCB-A55E-32DFDD6BE6BC}" name="Repo" dataDxfId="17" dataCellStyle="Hyperlink">
+    <tableColumn id="9" xr3:uid="{4F45D914-640E-4DCB-A55E-32DFDD6BE6BC}" name="Repo" dataDxfId="19" dataCellStyle="Hyperlink">
       <calculatedColumnFormula>LEFT(F2, FIND("/releases", F2) - 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{82D64721-6A58-4E8F-B4CC-4E9A79C19880}" name="sourceFileName" dataDxfId="16">
+    <tableColumn id="10" xr3:uid="{82D64721-6A58-4E8F-B4CC-4E9A79C19880}" name="sourceFileName" dataDxfId="18">
       <calculatedColumnFormula>IF(H2&lt;&gt;"", H2, RIGHT(F2,LEN(F2)-FIND("@",SUBSTITUTE(F2,"/","@",LEN(F2)-LEN(SUBSTITUTE(F2,"/",""))))))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3400,14 +3438,14 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:M155"/>
+  <dimension ref="A1:M156"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F135" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="F146" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
-      <selection pane="bottomRight" activeCell="K153" sqref="K153"/>
+      <selection pane="bottomRight" activeCell="I157" sqref="I157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -6384,20 +6422,37 @@
         <v>845</v>
       </c>
     </row>
+    <row r="156" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="E156" t="s">
+        <v>875</v>
+      </c>
+      <c r="F156">
+        <v>228696</v>
+      </c>
+      <c r="G156">
+        <v>2272531</v>
+      </c>
+      <c r="I156" t="s">
+        <v>396</v>
+      </c>
+      <c r="M156" s="4" t="s">
+        <v>876</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="I1:J98 I156:J1048576">
-    <cfRule type="cellIs" dxfId="15" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="7" operator="equal">
       <formula>"Custom License"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="8" operator="equal">
       <formula>"All Rights Reserved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I101:J155">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
       <formula>"Custom License"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
       <formula>"All Rights Reserved"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6507,12 +6562,12 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:O119"/>
+  <dimension ref="A1:O120"/>
   <sheetViews>
     <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="F55" sqref="F55"/>
+      <selection pane="bottomLeft" activeCell="E121" sqref="E121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -8209,7 +8264,7 @@
         <v>480</v>
       </c>
       <c r="M94" s="4" t="e">
-        <f t="shared" ref="M94:M118" si="6">LEFT(F94, FIND("/releases", F94) - 1)</f>
+        <f t="shared" ref="M94:M120" si="6">LEFT(F94, FIND("/releases", F94) - 1)</f>
         <v>#VALUE!</v>
       </c>
       <c r="N94" t="str">
@@ -8668,17 +8723,37 @@
       <c r="H119" t="s">
         <v>686</v>
       </c>
+      <c r="M119" s="4" t="e">
+        <f t="shared" si="6"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="N119" t="str">
         <f t="shared" si="7"/>
         <v>ztech1.7.10-0.0.3.jar</v>
       </c>
     </row>
+    <row r="120" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="E120" t="s">
+        <v>873</v>
+      </c>
+      <c r="F120" s="4" t="s">
+        <v>874</v>
+      </c>
+      <c r="M120" s="4" t="e">
+        <f t="shared" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N120" t="str">
+        <f>IF(H120&lt;&gt;"", H120, RIGHT(F120,LEN(F120)-FIND("@",SUBSTITUTE(F120,"/","@",LEN(F120)-LEN(SUBSTITUTE(F120,"/",""))))))</f>
+        <v>Technomancy - 0.12.5 - 1.7.10.jar</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="J3">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
       <formula>"Custom License"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
       <formula>"All Rights Reserved"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8811,14 +8886,14 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:M28"/>
+  <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="5" ySplit="1" topLeftCell="F11" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
-      <selection pane="bottomRight" activeCell="I28" sqref="I28"/>
+      <selection pane="bottomRight" activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -9418,19 +9493,42 @@
         <v>871</v>
       </c>
     </row>
+    <row r="29" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="E29" t="s">
+        <v>877</v>
+      </c>
+      <c r="F29">
+        <v>72503</v>
+      </c>
+      <c r="G29">
+        <v>2272713</v>
+      </c>
+      <c r="I29" t="s">
+        <v>396</v>
+      </c>
+      <c r="L29" t="s">
+        <v>879</v>
+      </c>
+      <c r="M29" s="4" t="s">
+        <v>878</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="I1:I28 I30:I1048576">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+  <conditionalFormatting sqref="I1:I1048576">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>"Custom License"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
       <formula>"All Rights Reserved"</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="M29" r:id="rId1" xr:uid="{DEF57671-F743-42F8-9DB0-CB7BB6AC7F63}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -9905,7 +10003,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10075,9 +10173,15 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C13" s="4" t="e">
+      <c r="A13">
+        <v>2295819</v>
+      </c>
+      <c r="B13" t="s">
+        <v>872</v>
+      </c>
+      <c r="C13" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>https://mediafilez.forgecdn.net/files/2295/819/Technomancy - 0.12.5 - 1.7.10.jar</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -10424,34 +10528,34 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E6:E18">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
       <formula>"Custom License"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
       <formula>"All Rights Reserved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20:E22">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
       <formula>"Custom License"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
       <formula>"All Rights Reserved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19:F19">
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"Custom License"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>"All Rights Reserved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23:F23">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"Custom License"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"All Rights Reserved"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
HUGE IC2 Quests Page (62 quests), added Technomancy
</commit_message>
<xml_diff>
--- a/config/mod-director/bundle.json v5.xlsx
+++ b/config/mod-director/bundle.json v5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason\AppData\Roaming\PrismLauncher\instances\Volentus FileDirector\minecraft\config\mod-director\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92710FFA-F579-43CE-B8D0-4FAD65564543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE578BF2-DC1B-43B0-866E-1FB9E2BA174E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1332" yWindow="216" windowWidth="22392" windowHeight="12024" tabRatio="839" activeTab="3" xr2:uid="{9C62C9EC-1015-4AFA-B33E-B214A55E5F8C}"/>
+    <workbookView xWindow="372" yWindow="216" windowWidth="22392" windowHeight="12024" tabRatio="839" xr2:uid="{9C62C9EC-1015-4AFA-B33E-B214A55E5F8C}"/>
   </bookViews>
   <sheets>
     <sheet name="CurseForge" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1202" uniqueCount="880">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1195" uniqueCount="875">
   <si>
     <t>addonId</t>
   </si>
@@ -2668,21 +2668,6 @@
   </si>
   <si>
     <t>https://mediafilez.forgecdn.net/files/2295/819/Technomancy - 0.12.5 - 1.7.10.jar</t>
-  </si>
-  <si>
-    <t>Thaumic Expansion</t>
-  </si>
-  <si>
-    <t>https://www.curseforge.com/minecraft/mc-mods/thaumic-expansion</t>
-  </si>
-  <si>
-    <t>Origin</t>
-  </si>
-  <si>
-    <t>https://www.curseforge.com/minecraft/mc-mods/origin</t>
-  </si>
-  <si>
-    <t>Origin-1.7.10-8.0.3.jar</t>
   </si>
 </sst>
 </file>
@@ -2805,21 +2790,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6565"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="23">
     <dxf>
       <fill>
         <patternFill>
@@ -3037,8 +3008,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CF71CB59-A681-467E-A496-DF22C8F63C36}" name="Table1" displayName="Table1" ref="A1:M156" totalsRowShown="0" headerRowDxfId="24">
-  <autoFilter ref="A1:M156" xr:uid="{CF71CB59-A681-467E-A496-DF22C8F63C36}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CF71CB59-A681-467E-A496-DF22C8F63C36}" name="Table1" displayName="Table1" ref="A1:M155" totalsRowShown="0" headerRowDxfId="22">
+  <autoFilter ref="A1:M155" xr:uid="{CF71CB59-A681-467E-A496-DF22C8F63C36}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L80">
     <sortCondition ref="E1:E80"/>
   </sortState>
@@ -3073,7 +3044,7 @@
     <tableColumn id="8" xr3:uid="{071FB076-79DA-4271-9B11-D3DAF5A27A08}" name="selectedByDefault"/>
     <tableColumn id="9" xr3:uid="{3CDEFED8-BDC9-47C7-831C-532778102D77}" name="description"/>
     <tableColumn id="1" xr3:uid="{E6FB84AB-CA8F-4CC7-B1A7-BC7A68F80D0F}" name="name"/>
-    <tableColumn id="2" xr3:uid="{F0A7EA2F-C2AC-43F5-BC6D-C49D0647EFC8}" name="url" dataDxfId="23" dataCellStyle="Hyperlink"/>
+    <tableColumn id="2" xr3:uid="{F0A7EA2F-C2AC-43F5-BC6D-C49D0647EFC8}" name="url" dataDxfId="21" dataCellStyle="Hyperlink"/>
     <tableColumn id="6" xr3:uid="{EC64C9C3-AEEF-4EBD-8BFF-4E2922D06865}" name="side"/>
     <tableColumn id="4" xr3:uid="{9F48CDE4-D924-41EA-B9F4-C5D89CD73B03}" name="fileName"/>
     <tableColumn id="5" xr3:uid="{7F05F574-DA53-49C9-8050-3D2CCDAB677A}" name="follows"/>
@@ -3081,7 +3052,7 @@
     <tableColumn id="11" xr3:uid="{D819B850-F57B-498C-825C-8A486975641F}" name="Notes"/>
     <tableColumn id="12" xr3:uid="{49D1682B-534D-4059-A5DA-B3CA78E5F4FB}" name="folder"/>
     <tableColumn id="13" xr3:uid="{4E3663E0-B283-45F0-9C3F-F05498D5CFFD}" name="Repo" dataCellStyle="Hyperlink"/>
-    <tableColumn id="14" xr3:uid="{D8C83F8D-C674-4041-9191-44B2463F4BF7}" name="sourceFileName" dataDxfId="22">
+    <tableColumn id="14" xr3:uid="{D8C83F8D-C674-4041-9191-44B2463F4BF7}" name="sourceFileName" dataDxfId="20">
       <calculatedColumnFormula>IF(H2&lt;&gt;"", H2, RIGHT(F2,LEN(F2)-FIND("@",SUBSTITUTE(F2,"/","@",LEN(F2)-LEN(SUBSTITUTE(F2,"/",""))))))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="15" xr3:uid="{AC8070E0-756B-431E-A1EC-4CB67F73C9E2}" name="followsIL"/>
@@ -3091,8 +3062,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{837A1DAE-8158-4E48-816C-7B02D8E95473}" name="Table6" displayName="Table6" ref="A1:M29" totalsRowShown="0" headerRowDxfId="21">
-  <autoFilter ref="A1:M29" xr:uid="{837A1DAE-8158-4E48-816C-7B02D8E95473}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{837A1DAE-8158-4E48-816C-7B02D8E95473}" name="Table6" displayName="Table6" ref="A1:M28" totalsRowShown="0" headerRowDxfId="19">
+  <autoFilter ref="A1:M28" xr:uid="{837A1DAE-8158-4E48-816C-7B02D8E95473}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L28">
     <sortCondition ref="E1:E28"/>
   </sortState>
@@ -3120,17 +3091,17 @@
   <autoFilter ref="E1:N13" xr:uid="{8FA21BC5-EE0E-4191-BC63-9EB4198DCDF8}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{60D5533B-280C-4133-820D-E94C6E9E36DB}" name="name"/>
-    <tableColumn id="2" xr3:uid="{66EF7A2B-9A21-4085-93F7-14CD58F6F15B}" name="url" dataDxfId="20" dataCellStyle="Hyperlink"/>
+    <tableColumn id="2" xr3:uid="{66EF7A2B-9A21-4085-93F7-14CD58F6F15B}" name="url" dataDxfId="18" dataCellStyle="Hyperlink"/>
     <tableColumn id="3" xr3:uid="{C0731F1D-4A65-4CA3-9F35-0689AF888300}" name="side"/>
     <tableColumn id="4" xr3:uid="{20970281-086F-4DD1-BF01-7E06711A2DDF}" name="fileName"/>
     <tableColumn id="5" xr3:uid="{B177552A-E452-47D5-80D6-29CB46C2F510}" name="follows"/>
     <tableColumn id="6" xr3:uid="{1962D553-6A3F-4CA6-927C-7A94E4C9757F}" name="License"/>
     <tableColumn id="7" xr3:uid="{48F547D9-B9D6-48B9-BAA7-B1972742C050}" name="Notes"/>
     <tableColumn id="8" xr3:uid="{948716AE-E46C-40AC-A5A6-5231FDD8884A}" name="folder"/>
-    <tableColumn id="9" xr3:uid="{4F45D914-640E-4DCB-A55E-32DFDD6BE6BC}" name="Repo" dataDxfId="19" dataCellStyle="Hyperlink">
+    <tableColumn id="9" xr3:uid="{4F45D914-640E-4DCB-A55E-32DFDD6BE6BC}" name="Repo" dataDxfId="17" dataCellStyle="Hyperlink">
       <calculatedColumnFormula>LEFT(F2, FIND("/releases", F2) - 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{82D64721-6A58-4E8F-B4CC-4E9A79C19880}" name="sourceFileName" dataDxfId="18">
+    <tableColumn id="10" xr3:uid="{82D64721-6A58-4E8F-B4CC-4E9A79C19880}" name="sourceFileName" dataDxfId="16">
       <calculatedColumnFormula>IF(H2&lt;&gt;"", H2, RIGHT(F2,LEN(F2)-FIND("@",SUBSTITUTE(F2,"/","@",LEN(F2)-LEN(SUBSTITUTE(F2,"/",""))))))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3438,14 +3409,14 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:M156"/>
+  <dimension ref="A1:M155"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F146" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="F137" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
-      <selection pane="bottomRight" activeCell="I157" sqref="I157"/>
+      <selection pane="bottomRight" activeCell="L151" sqref="L151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -6422,44 +6393,30 @@
         <v>845</v>
       </c>
     </row>
-    <row r="156" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E156" t="s">
-        <v>875</v>
-      </c>
-      <c r="F156">
-        <v>228696</v>
-      </c>
-      <c r="G156">
-        <v>2272531</v>
-      </c>
-      <c r="I156" t="s">
-        <v>396</v>
-      </c>
-      <c r="M156" s="4" t="s">
-        <v>876</v>
-      </c>
-    </row>
   </sheetData>
   <conditionalFormatting sqref="I1:J98 I156:J1048576">
-    <cfRule type="cellIs" dxfId="17" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="7" operator="equal">
       <formula>"Custom License"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="8" operator="equal">
       <formula>"All Rights Reserved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I101:J155">
-    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
       <formula>"Custom License"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
       <formula>"All Rights Reserved"</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="M153" r:id="rId1" xr:uid="{0297EA0E-AABC-42E6-BD9C-C92D40E3D114}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -8750,10 +8707,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J3">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>"Custom License"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
       <formula>"All Rights Reserved"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8886,14 +8843,14 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:M29"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="5" ySplit="1" topLeftCell="F11" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
-      <selection pane="bottomRight" activeCell="L30" sqref="L30"/>
+      <selection pane="bottomRight" activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -9493,42 +9450,19 @@
         <v>871</v>
       </c>
     </row>
-    <row r="29" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E29" t="s">
-        <v>877</v>
-      </c>
-      <c r="F29">
-        <v>72503</v>
-      </c>
-      <c r="G29">
-        <v>2272713</v>
-      </c>
-      <c r="I29" t="s">
-        <v>396</v>
-      </c>
-      <c r="L29" t="s">
-        <v>879</v>
-      </c>
-      <c r="M29" s="4" t="s">
-        <v>878</v>
-      </c>
-    </row>
   </sheetData>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>"Custom License"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
       <formula>"All Rights Reserved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <hyperlinks>
-    <hyperlink ref="M29" r:id="rId1" xr:uid="{DEF57671-F743-42F8-9DB0-CB7BB6AC7F63}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -10528,34 +10462,34 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E6:E18">
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>"Custom License"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
       <formula>"All Rights Reserved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20:E22">
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>"Custom License"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"All Rights Reserved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19:F19">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>"Custom License"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
       <formula>"All Rights Reserved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23:F23">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Custom License"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"All Rights Reserved"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added Adjachest, some quest updates (FTA)
</commit_message>
<xml_diff>
--- a/config/mod-director/bundle.json v5.xlsx
+++ b/config/mod-director/bundle.json v5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason\AppData\Roaming\PrismLauncher\instances\Volentus FileDirector\minecraft\config\mod-director\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B21F213-2A07-40D1-94D8-54E0EA400B35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27714A76-D46D-4866-81C9-50BE3D1B535B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="372" yWindow="216" windowWidth="22392" windowHeight="12024" tabRatio="839" activeTab="8" xr2:uid="{9C62C9EC-1015-4AFA-B33E-B214A55E5F8C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="839" xr2:uid="{9C62C9EC-1015-4AFA-B33E-B214A55E5F8C}"/>
   </bookViews>
   <sheets>
     <sheet name="CurseForge" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1222" uniqueCount="883">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1234" uniqueCount="891">
   <si>
     <t>addonId</t>
   </si>
@@ -2692,6 +2692,30 @@
   </si>
   <si>
     <t>Not needed</t>
+  </si>
+  <si>
+    <t>Adjachest</t>
+  </si>
+  <si>
+    <t>https://github.com/Myask-sl/adjachest-1.7.10/releases/download/v0.9.9.9beta10/adjachest-0.9.9.9beta10.jar</t>
+  </si>
+  <si>
+    <t>Beddium</t>
+  </si>
+  <si>
+    <t>FalseTweaks</t>
+  </si>
+  <si>
+    <t>https://www.curseforge.com/minecraft/mc-mods/beddium</t>
+  </si>
+  <si>
+    <t>https://www.curseforge.com/minecraft/mc-mods/falsetweaks</t>
+  </si>
+  <si>
+    <t>FalsePatternLib</t>
+  </si>
+  <si>
+    <t>https://www.curseforge.com/minecraft/mc-mods/fplib</t>
   </si>
 </sst>
 </file>
@@ -2806,7 +2830,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2827,14 +2851,104 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="39">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6565"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6565"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6565"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6565"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6565"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6565"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3080,10 +3194,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CF71CB59-A681-467E-A496-DF22C8F63C36}" name="Table1" displayName="Table1" ref="A1:M155" totalsRowShown="0" headerRowDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CF71CB59-A681-467E-A496-DF22C8F63C36}" name="Table1" displayName="Table1" ref="A1:M155" totalsRowShown="0" headerRowDxfId="38">
   <autoFilter ref="A1:M155" xr:uid="{CF71CB59-A681-467E-A496-DF22C8F63C36}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L80">
-    <sortCondition ref="E1:E80"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L79">
+    <sortCondition ref="E1:E79"/>
   </sortState>
   <tableColumns count="13">
     <tableColumn id="9" xr3:uid="{34883474-1328-4AD0-B92C-8AFF0A9B4D2F}" name="continueOnFailedDownload"/>
@@ -3105,8 +3219,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8C69A2DD-805E-41CC-A56E-3CB65AD41149}" name="Table2" displayName="Table2" ref="A1:O119" totalsRowShown="0">
-  <autoFilter ref="A1:O119" xr:uid="{8C69A2DD-805E-41CC-A56E-3CB65AD41149}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8C69A2DD-805E-41CC-A56E-3CB65AD41149}" name="Table2" displayName="Table2" ref="A1:O120" totalsRowShown="0">
+  <autoFilter ref="A1:O120" xr:uid="{8C69A2DD-805E-41CC-A56E-3CB65AD41149}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E2:I28">
     <sortCondition ref="E1:E28"/>
   </sortState>
@@ -3116,7 +3230,7 @@
     <tableColumn id="8" xr3:uid="{071FB076-79DA-4271-9B11-D3DAF5A27A08}" name="selectedByDefault"/>
     <tableColumn id="9" xr3:uid="{3CDEFED8-BDC9-47C7-831C-532778102D77}" name="description"/>
     <tableColumn id="1" xr3:uid="{E6FB84AB-CA8F-4CC7-B1A7-BC7A68F80D0F}" name="name"/>
-    <tableColumn id="2" xr3:uid="{F0A7EA2F-C2AC-43F5-BC6D-C49D0647EFC8}" name="url" dataDxfId="25" dataCellStyle="Hyperlink"/>
+    <tableColumn id="2" xr3:uid="{F0A7EA2F-C2AC-43F5-BC6D-C49D0647EFC8}" name="url" dataDxfId="37" dataCellStyle="Hyperlink"/>
     <tableColumn id="6" xr3:uid="{EC64C9C3-AEEF-4EBD-8BFF-4E2922D06865}" name="side"/>
     <tableColumn id="4" xr3:uid="{9F48CDE4-D924-41EA-B9F4-C5D89CD73B03}" name="fileName"/>
     <tableColumn id="5" xr3:uid="{7F05F574-DA53-49C9-8050-3D2CCDAB677A}" name="follows"/>
@@ -3124,7 +3238,7 @@
     <tableColumn id="11" xr3:uid="{D819B850-F57B-498C-825C-8A486975641F}" name="Notes"/>
     <tableColumn id="12" xr3:uid="{49D1682B-534D-4059-A5DA-B3CA78E5F4FB}" name="folder"/>
     <tableColumn id="13" xr3:uid="{4E3663E0-B283-45F0-9C3F-F05498D5CFFD}" name="Repo" dataCellStyle="Hyperlink"/>
-    <tableColumn id="14" xr3:uid="{D8C83F8D-C674-4041-9191-44B2463F4BF7}" name="sourceFileName" dataDxfId="24">
+    <tableColumn id="14" xr3:uid="{D8C83F8D-C674-4041-9191-44B2463F4BF7}" name="sourceFileName" dataDxfId="36">
       <calculatedColumnFormula>IF(H2&lt;&gt;"", H2, RIGHT(F2,LEN(F2)-FIND("@",SUBSTITUTE(F2,"/","@",LEN(F2)-LEN(SUBSTITUTE(F2,"/",""))))))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="15" xr3:uid="{AC8070E0-756B-431E-A1EC-4CB67F73C9E2}" name="followsIL"/>
@@ -3134,8 +3248,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{837A1DAE-8158-4E48-816C-7B02D8E95473}" name="Table6" displayName="Table6" ref="A1:M28" totalsRowShown="0" headerRowDxfId="23">
-  <autoFilter ref="A1:M28" xr:uid="{837A1DAE-8158-4E48-816C-7B02D8E95473}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{837A1DAE-8158-4E48-816C-7B02D8E95473}" name="Table6" displayName="Table6" ref="A1:M29" totalsRowShown="0" headerRowDxfId="35">
+  <autoFilter ref="A1:M29" xr:uid="{837A1DAE-8158-4E48-816C-7B02D8E95473}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L28">
     <sortCondition ref="E1:E28"/>
   </sortState>
@@ -3163,17 +3277,17 @@
   <autoFilter ref="E1:N13" xr:uid="{8FA21BC5-EE0E-4191-BC63-9EB4198DCDF8}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{60D5533B-280C-4133-820D-E94C6E9E36DB}" name="name"/>
-    <tableColumn id="2" xr3:uid="{66EF7A2B-9A21-4085-93F7-14CD58F6F15B}" name="url" dataDxfId="22" dataCellStyle="Hyperlink"/>
+    <tableColumn id="2" xr3:uid="{66EF7A2B-9A21-4085-93F7-14CD58F6F15B}" name="url" dataDxfId="34" dataCellStyle="Hyperlink"/>
     <tableColumn id="3" xr3:uid="{C0731F1D-4A65-4CA3-9F35-0689AF888300}" name="side"/>
     <tableColumn id="4" xr3:uid="{20970281-086F-4DD1-BF01-7E06711A2DDF}" name="fileName"/>
     <tableColumn id="5" xr3:uid="{B177552A-E452-47D5-80D6-29CB46C2F510}" name="follows"/>
     <tableColumn id="6" xr3:uid="{1962D553-6A3F-4CA6-927C-7A94E4C9757F}" name="License"/>
     <tableColumn id="7" xr3:uid="{48F547D9-B9D6-48B9-BAA7-B1972742C050}" name="Notes"/>
     <tableColumn id="8" xr3:uid="{948716AE-E46C-40AC-A5A6-5231FDD8884A}" name="folder"/>
-    <tableColumn id="9" xr3:uid="{4F45D914-640E-4DCB-A55E-32DFDD6BE6BC}" name="Repo" dataDxfId="21" dataCellStyle="Hyperlink">
+    <tableColumn id="9" xr3:uid="{4F45D914-640E-4DCB-A55E-32DFDD6BE6BC}" name="Repo" dataDxfId="33" dataCellStyle="Hyperlink">
       <calculatedColumnFormula>LEFT(F2, FIND("/releases", F2) - 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{82D64721-6A58-4E8F-B4CC-4E9A79C19880}" name="sourceFileName" dataDxfId="20">
+    <tableColumn id="10" xr3:uid="{82D64721-6A58-4E8F-B4CC-4E9A79C19880}" name="sourceFileName" dataDxfId="32">
       <calculatedColumnFormula>IF(H2&lt;&gt;"", H2, RIGHT(F2,LEN(F2)-FIND("@",SUBSTITUTE(F2,"/","@",LEN(F2)-LEN(SUBSTITUTE(F2,"/",""))))))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3483,12 +3597,12 @@
   </sheetPr>
   <dimension ref="A1:M155"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="F138" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
-      <selection pane="bottomRight" activeCell="E1" sqref="E1:M1"/>
+      <selection pane="bottomRight" activeCell="E155" sqref="E155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -4394,2096 +4508,2107 @@
     </row>
     <row r="44" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E44" t="s">
-        <v>34</v>
+        <v>161</v>
       </c>
       <c r="F44">
-        <v>1031274</v>
+        <v>66675</v>
       </c>
       <c r="G44">
-        <v>6039947</v>
+        <v>2369671</v>
       </c>
       <c r="I44" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
       <c r="L44" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="M44" s="4" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
     </row>
     <row r="45" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E45" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F45">
-        <v>66675</v>
+        <v>533411</v>
       </c>
       <c r="G45">
-        <v>2369671</v>
+        <v>3479729</v>
       </c>
       <c r="I45" t="s">
-        <v>241</v>
+        <v>261</v>
       </c>
       <c r="L45" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="M45" s="4" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
     </row>
     <row r="46" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E46" t="s">
-        <v>162</v>
+        <v>242</v>
       </c>
       <c r="F46">
-        <v>533411</v>
+        <v>358228</v>
       </c>
       <c r="G46">
-        <v>3479729</v>
+        <v>6989739</v>
       </c>
       <c r="I46" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="L46" t="s">
-        <v>602</v>
+        <v>683</v>
       </c>
       <c r="M46" s="4" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
     </row>
     <row r="47" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E47" t="s">
-        <v>242</v>
+        <v>164</v>
       </c>
       <c r="F47">
-        <v>358228</v>
+        <v>225815</v>
       </c>
       <c r="G47">
-        <v>6989739</v>
+        <v>2323485</v>
       </c>
       <c r="I47" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="L47" t="s">
-        <v>683</v>
+        <v>603</v>
       </c>
       <c r="M47" s="4" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
     </row>
     <row r="48" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E48" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="F48">
-        <v>225815</v>
+        <v>228818</v>
       </c>
       <c r="G48">
-        <v>2323485</v>
+        <v>2386738</v>
       </c>
       <c r="I48" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="L48" t="s">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c r="M48" s="4" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
     </row>
     <row r="49" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E49" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F49">
-        <v>228818</v>
+        <v>228819</v>
       </c>
       <c r="G49">
-        <v>2386738</v>
+        <v>2386741</v>
       </c>
       <c r="I49" t="s">
         <v>257</v>
       </c>
       <c r="L49" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="M49" s="4" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
     </row>
     <row r="50" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E50" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F50">
-        <v>228819</v>
+        <v>221857</v>
       </c>
       <c r="G50">
-        <v>2386741</v>
+        <v>2270206</v>
       </c>
       <c r="I50" t="s">
-        <v>257</v>
+        <v>241</v>
       </c>
       <c r="L50" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="M50" s="4" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
     </row>
     <row r="51" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E51" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F51">
-        <v>221857</v>
+        <v>226687</v>
       </c>
       <c r="G51">
-        <v>2270206</v>
+        <v>2286103</v>
       </c>
       <c r="I51" t="s">
-        <v>241</v>
+        <v>258</v>
       </c>
       <c r="L51" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="M51" s="4" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
     </row>
     <row r="52" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E52" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="F52">
-        <v>226687</v>
+        <v>229084</v>
       </c>
       <c r="G52">
-        <v>2286103</v>
+        <v>2480016</v>
       </c>
       <c r="I52" t="s">
-        <v>258</v>
+        <v>241</v>
       </c>
       <c r="L52" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="M52" s="4" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
     </row>
     <row r="53" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E53" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F53">
-        <v>229084</v>
+        <v>225064</v>
       </c>
       <c r="G53">
-        <v>2480016</v>
+        <v>2263111</v>
       </c>
       <c r="I53" t="s">
-        <v>241</v>
+        <v>254</v>
       </c>
       <c r="L53" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="M53" s="4" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
     </row>
     <row r="54" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E54" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="F54">
-        <v>225064</v>
+        <v>240562</v>
       </c>
       <c r="G54">
-        <v>2263111</v>
+        <v>2306263</v>
       </c>
       <c r="I54" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="L54" t="s">
-        <v>610</v>
+        <v>641</v>
       </c>
       <c r="M54" s="4" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
     </row>
     <row r="55" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E55" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
       <c r="F55">
-        <v>240562</v>
+        <v>231935</v>
       </c>
       <c r="G55">
-        <v>2306263</v>
+        <v>2271259</v>
       </c>
       <c r="I55" t="s">
         <v>241</v>
       </c>
       <c r="L55" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="M55" s="4" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
     </row>
     <row r="56" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E56" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F56">
-        <v>231935</v>
+        <v>228609</v>
       </c>
       <c r="G56">
-        <v>2271259</v>
+        <v>2272589</v>
       </c>
       <c r="I56" t="s">
-        <v>241</v>
+        <v>254</v>
       </c>
       <c r="L56" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="M56" s="4" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
     </row>
     <row r="57" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E57" t="s">
-        <v>193</v>
+        <v>90</v>
       </c>
       <c r="F57">
-        <v>228609</v>
+        <v>235593</v>
       </c>
       <c r="G57">
-        <v>2272589</v>
+        <v>4721203</v>
       </c>
       <c r="I57" t="s">
         <v>254</v>
       </c>
       <c r="L57" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="M57" s="4" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
     </row>
     <row r="58" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E58" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="F58">
-        <v>235593</v>
+        <v>533411</v>
       </c>
       <c r="G58">
-        <v>4721203</v>
+        <v>3479729</v>
       </c>
       <c r="I58" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="L58" t="s">
-        <v>644</v>
+        <v>602</v>
       </c>
       <c r="M58" s="4" t="s">
-        <v>749</v>
+        <v>737</v>
       </c>
     </row>
     <row r="59" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E59" t="s">
-        <v>108</v>
+        <v>199</v>
       </c>
       <c r="F59">
-        <v>533411</v>
+        <v>70631</v>
       </c>
       <c r="G59">
-        <v>3479729</v>
+        <v>2277490</v>
       </c>
       <c r="I59" t="s">
-        <v>261</v>
+        <v>241</v>
       </c>
       <c r="L59" t="s">
-        <v>602</v>
+        <v>645</v>
       </c>
       <c r="M59" s="4" t="s">
-        <v>737</v>
+        <v>750</v>
       </c>
     </row>
     <row r="60" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E60" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F60">
-        <v>70631</v>
+        <v>75811</v>
       </c>
       <c r="G60">
-        <v>2277490</v>
+        <v>2393121</v>
       </c>
       <c r="I60" t="s">
-        <v>241</v>
+        <v>255</v>
       </c>
       <c r="L60" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="M60" s="4" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
     </row>
     <row r="61" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E61" t="s">
-        <v>200</v>
+        <v>284</v>
       </c>
       <c r="F61">
-        <v>75811</v>
+        <v>241319</v>
       </c>
       <c r="G61">
-        <v>2393121</v>
+        <v>2323453</v>
       </c>
       <c r="I61" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="L61" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="M61" s="4" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
     </row>
     <row r="62" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E62" t="s">
-        <v>284</v>
+        <v>201</v>
       </c>
       <c r="F62">
-        <v>241319</v>
+        <v>224641</v>
       </c>
       <c r="G62">
-        <v>2323453</v>
+        <v>2287287</v>
       </c>
       <c r="I62" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="L62" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="M62" s="4" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="63" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E63" t="s">
-        <v>201</v>
+        <v>91</v>
       </c>
       <c r="F63">
-        <v>224641</v>
+        <v>235596</v>
       </c>
       <c r="G63">
-        <v>2287287</v>
+        <v>4721191</v>
       </c>
       <c r="I63" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="L63" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="M63" s="4" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
     </row>
     <row r="64" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E64" t="s">
-        <v>91</v>
+        <v>202</v>
       </c>
       <c r="F64">
-        <v>235596</v>
+        <v>223808</v>
       </c>
       <c r="G64">
-        <v>4721191</v>
+        <v>2320429</v>
       </c>
       <c r="I64" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="L64" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="M64" s="4" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
     </row>
     <row r="65" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E65" t="s">
-        <v>202</v>
+        <v>73</v>
       </c>
       <c r="F65">
-        <v>223808</v>
+        <v>223722</v>
       </c>
       <c r="G65">
-        <v>2320429</v>
+        <v>2299730</v>
       </c>
       <c r="I65" t="s">
         <v>241</v>
       </c>
       <c r="L65" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="M65" s="4" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
     </row>
     <row r="66" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E66" t="s">
-        <v>73</v>
+        <v>203</v>
       </c>
       <c r="F66">
-        <v>223722</v>
+        <v>290114</v>
       </c>
       <c r="G66">
-        <v>2299730</v>
+        <v>2541028</v>
       </c>
       <c r="I66" t="s">
-        <v>241</v>
+        <v>257</v>
       </c>
       <c r="L66" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="M66" s="4" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
     </row>
     <row r="67" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E67" t="s">
-        <v>203</v>
+        <v>37</v>
       </c>
       <c r="F67">
-        <v>290114</v>
+        <v>223628</v>
       </c>
       <c r="G67">
-        <v>2541028</v>
+        <v>2227552</v>
       </c>
       <c r="I67" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="L67" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="M67" s="4" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
     </row>
     <row r="68" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E68" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="F68">
-        <v>223628</v>
+        <v>431297</v>
       </c>
       <c r="G68">
-        <v>2227552</v>
+        <v>6929888</v>
       </c>
       <c r="I68" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="L68" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="M68" s="4" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
     </row>
     <row r="69" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E69" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="F69">
-        <v>431297</v>
+        <v>225095</v>
       </c>
       <c r="G69">
-        <v>6929888</v>
+        <v>2241913</v>
       </c>
       <c r="I69" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="L69" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="M69" s="4" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
     </row>
     <row r="70" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E70" t="s">
-        <v>65</v>
+        <v>38</v>
       </c>
       <c r="F70">
-        <v>225095</v>
+        <v>227443</v>
       </c>
       <c r="G70">
-        <v>2241913</v>
+        <v>2388756</v>
       </c>
       <c r="I70" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="L70" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="M70" s="4" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
     </row>
     <row r="71" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E71" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F71">
-        <v>227443</v>
+        <v>69163</v>
       </c>
       <c r="G71">
-        <v>2388756</v>
+        <v>2388758</v>
       </c>
       <c r="I71" t="s">
         <v>241</v>
       </c>
       <c r="L71" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="M71" s="4" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
     </row>
     <row r="72" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E72" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F72">
-        <v>69163</v>
+        <v>222880</v>
       </c>
       <c r="G72">
-        <v>2388758</v>
+        <v>2388752</v>
       </c>
       <c r="I72" t="s">
         <v>241</v>
       </c>
       <c r="L72" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="M72" s="4" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
     </row>
     <row r="73" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E73" t="s">
-        <v>40</v>
+        <v>343</v>
       </c>
       <c r="F73">
-        <v>222880</v>
+        <v>238603</v>
       </c>
       <c r="G73">
-        <v>2388752</v>
-      </c>
-      <c r="I73" t="s">
-        <v>241</v>
+        <v>2588365</v>
       </c>
       <c r="L73" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="M73" s="4" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
     </row>
     <row r="74" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E74" t="s">
-        <v>343</v>
+        <v>92</v>
       </c>
       <c r="F74">
-        <v>238603</v>
+        <v>347551</v>
       </c>
       <c r="G74">
-        <v>2588365</v>
+        <v>4721206</v>
+      </c>
+      <c r="I74" t="s">
+        <v>254</v>
+      </c>
+      <c r="K74" t="s">
+        <v>267</v>
       </c>
       <c r="L74" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="M74" s="4" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
     </row>
     <row r="75" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E75" t="s">
-        <v>92</v>
+        <v>24</v>
       </c>
       <c r="F75">
-        <v>347551</v>
+        <v>826970</v>
       </c>
       <c r="G75">
-        <v>4721206</v>
+        <v>6761003</v>
       </c>
       <c r="I75" t="s">
         <v>254</v>
       </c>
-      <c r="K75" t="s">
-        <v>267</v>
-      </c>
       <c r="L75" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="M75" s="4" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
     </row>
     <row r="76" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E76" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="F76">
-        <v>826970</v>
+        <v>235612</v>
       </c>
       <c r="G76">
-        <v>6761003</v>
+        <v>4721207</v>
       </c>
       <c r="I76" t="s">
         <v>254</v>
       </c>
+      <c r="K76" t="s">
+        <v>267</v>
+      </c>
       <c r="L76" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="M76" s="4" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
     </row>
     <row r="77" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E77" t="s">
-        <v>93</v>
+        <v>64</v>
       </c>
       <c r="F77">
-        <v>235612</v>
+        <v>229625</v>
       </c>
       <c r="G77">
-        <v>4721207</v>
+        <v>2263163</v>
+      </c>
+      <c r="H77" t="s">
+        <v>250</v>
       </c>
       <c r="I77" t="s">
         <v>254</v>
       </c>
-      <c r="K77" t="s">
-        <v>267</v>
-      </c>
       <c r="L77" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="M77" s="4" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
     </row>
     <row r="78" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E78" t="s">
-        <v>64</v>
+        <v>17</v>
       </c>
       <c r="F78">
-        <v>229625</v>
+        <v>69673</v>
       </c>
       <c r="G78">
-        <v>2263163</v>
-      </c>
-      <c r="H78" t="s">
-        <v>250</v>
+        <v>2234410</v>
       </c>
       <c r="I78" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="L78" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="M78" s="4" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
     </row>
     <row r="79" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E79" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F79">
-        <v>69673</v>
+        <v>253015</v>
       </c>
       <c r="G79">
-        <v>2234410</v>
+        <v>2340610</v>
       </c>
       <c r="I79" t="s">
-        <v>241</v>
+        <v>257</v>
       </c>
       <c r="L79" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="M79" s="4" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
     </row>
     <row r="80" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E80" t="s">
-        <v>16</v>
+        <v>354</v>
       </c>
       <c r="F80">
-        <v>253015</v>
+        <v>302569</v>
       </c>
       <c r="G80">
-        <v>2340610</v>
+        <v>2614309</v>
       </c>
       <c r="I80" t="s">
-        <v>257</v>
+        <v>295</v>
       </c>
       <c r="L80" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="M80" s="4" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
     </row>
     <row r="81" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E81" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="F81">
-        <v>302569</v>
+        <v>223622</v>
       </c>
       <c r="G81">
-        <v>2614309</v>
+        <v>2298965</v>
       </c>
       <c r="I81" t="s">
-        <v>295</v>
+        <v>257</v>
       </c>
       <c r="L81" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="M81" s="4" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
     </row>
     <row r="82" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E82" t="s">
-        <v>355</v>
+        <v>370</v>
       </c>
       <c r="F82">
-        <v>223622</v>
+        <v>225635</v>
       </c>
       <c r="G82">
-        <v>2298965</v>
+        <v>2284130</v>
       </c>
       <c r="I82" t="s">
         <v>257</v>
       </c>
       <c r="L82" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="M82" s="4" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
     </row>
     <row r="83" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E83" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="F83">
-        <v>225635</v>
+        <v>301924</v>
       </c>
       <c r="G83">
-        <v>2284130</v>
+        <v>2688012</v>
       </c>
       <c r="I83" t="s">
         <v>257</v>
       </c>
       <c r="L83" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="M83" s="4" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
     </row>
     <row r="84" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E84" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="F84">
-        <v>301924</v>
+        <v>237593</v>
       </c>
       <c r="G84">
-        <v>2688012</v>
+        <v>2299527</v>
       </c>
       <c r="I84" t="s">
-        <v>257</v>
+        <v>277</v>
       </c>
       <c r="L84" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="M84" s="4" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
     </row>
     <row r="85" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E85" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="F85">
-        <v>237593</v>
+        <v>228029</v>
       </c>
       <c r="G85">
-        <v>2299527</v>
+        <v>2282145</v>
       </c>
       <c r="I85" t="s">
-        <v>277</v>
+        <v>257</v>
       </c>
       <c r="L85" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="M85" s="4" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
     </row>
     <row r="86" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E86" t="s">
-        <v>382</v>
+        <v>392</v>
       </c>
       <c r="F86">
-        <v>228029</v>
+        <v>235544</v>
       </c>
       <c r="G86">
-        <v>2282145</v>
+        <v>2852697</v>
       </c>
       <c r="I86" t="s">
-        <v>257</v>
+        <v>241</v>
       </c>
       <c r="L86" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="M86" s="4" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
     </row>
     <row r="87" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E87" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="F87">
-        <v>235544</v>
+        <v>227099</v>
       </c>
       <c r="G87">
-        <v>2852697</v>
+        <v>2261766</v>
       </c>
       <c r="I87" t="s">
-        <v>241</v>
+        <v>257</v>
       </c>
       <c r="L87" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="M87" s="4" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
     </row>
     <row r="88" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E88" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="F88">
-        <v>227099</v>
+        <v>222153</v>
       </c>
       <c r="G88">
-        <v>2261766</v>
+        <v>2285272</v>
       </c>
       <c r="I88" t="s">
-        <v>257</v>
+        <v>241</v>
       </c>
       <c r="L88" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="M88" s="4" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
     </row>
     <row r="89" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E89" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="F89">
-        <v>222153</v>
+        <v>221457</v>
       </c>
       <c r="G89">
-        <v>2285272</v>
+        <v>2288782</v>
       </c>
       <c r="I89" t="s">
-        <v>241</v>
+        <v>396</v>
       </c>
       <c r="L89" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="M89" s="4" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
     </row>
     <row r="90" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E90" t="s">
-        <v>395</v>
+        <v>401</v>
       </c>
       <c r="F90">
-        <v>221457</v>
+        <v>223957</v>
       </c>
       <c r="G90">
-        <v>2288782</v>
+        <v>2772380</v>
       </c>
       <c r="I90" t="s">
-        <v>396</v>
+        <v>254</v>
       </c>
       <c r="L90" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="M90" s="4" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
     </row>
     <row r="91" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E91" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="F91">
-        <v>223957</v>
+        <v>256398</v>
       </c>
       <c r="G91">
-        <v>2772380</v>
+        <v>2694963</v>
       </c>
       <c r="I91" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="L91" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="M91" s="4" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
     </row>
     <row r="92" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E92" t="s">
-        <v>404</v>
+        <v>386</v>
       </c>
       <c r="F92">
-        <v>256398</v>
+        <v>60092</v>
       </c>
       <c r="G92">
-        <v>2694963</v>
+        <v>2219018</v>
       </c>
       <c r="I92" t="s">
-        <v>241</v>
+        <v>387</v>
       </c>
       <c r="L92" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="M92" s="4" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
     </row>
     <row r="93" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E93" t="s">
-        <v>386</v>
+        <v>409</v>
       </c>
       <c r="F93">
-        <v>60092</v>
+        <v>228027</v>
       </c>
       <c r="G93">
-        <v>2219018</v>
+        <v>2423369</v>
       </c>
       <c r="I93" t="s">
-        <v>387</v>
+        <v>241</v>
       </c>
       <c r="L93" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="M93" s="4" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
     </row>
     <row r="94" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E94" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="F94">
-        <v>228027</v>
+        <v>228364</v>
       </c>
       <c r="G94">
-        <v>2423369</v>
+        <v>2229581</v>
       </c>
       <c r="I94" t="s">
         <v>241</v>
       </c>
       <c r="L94" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="M94" s="4" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
     </row>
     <row r="95" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E95" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="F95">
-        <v>228364</v>
+        <v>228362</v>
       </c>
       <c r="G95">
-        <v>2229581</v>
+        <v>2229577</v>
       </c>
       <c r="I95" t="s">
         <v>241</v>
       </c>
       <c r="L95" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="M95" s="4" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
     </row>
     <row r="96" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E96" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="F96">
-        <v>228362</v>
+        <v>228363</v>
       </c>
       <c r="G96">
-        <v>2229577</v>
+        <v>2229574</v>
       </c>
       <c r="I96" t="s">
         <v>241</v>
       </c>
-      <c r="L96" t="s">
-        <v>681</v>
-      </c>
       <c r="M96" s="4" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
     </row>
     <row r="97" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E97" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="F97">
-        <v>228363</v>
+        <v>241994</v>
       </c>
       <c r="G97">
-        <v>2229574</v>
+        <v>2282591</v>
       </c>
       <c r="I97" t="s">
-        <v>241</v>
+        <v>257</v>
       </c>
       <c r="M97" s="4" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
     </row>
     <row r="98" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E98" t="s">
-        <v>413</v>
+        <v>397</v>
       </c>
       <c r="F98">
-        <v>241994</v>
+        <v>233785</v>
       </c>
       <c r="G98">
-        <v>2282591</v>
+        <v>2519595</v>
       </c>
       <c r="I98" t="s">
-        <v>257</v>
+        <v>283</v>
       </c>
       <c r="M98" s="4" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
     </row>
     <row r="99" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E99" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="F99">
-        <v>233785</v>
+        <v>248873</v>
       </c>
       <c r="G99">
-        <v>2519595</v>
+        <v>2502196</v>
       </c>
       <c r="I99" t="s">
-        <v>283</v>
+        <v>400</v>
       </c>
       <c r="M99" s="4" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
     </row>
     <row r="100" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E100" t="s">
-        <v>398</v>
+        <v>419</v>
       </c>
       <c r="F100">
-        <v>248873</v>
+        <v>238129</v>
       </c>
       <c r="G100">
-        <v>2502196</v>
+        <v>2309393</v>
       </c>
       <c r="I100" t="s">
-        <v>400</v>
+        <v>420</v>
+      </c>
+      <c r="K100" t="s">
+        <v>589</v>
       </c>
       <c r="M100" s="4" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
     </row>
     <row r="101" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E101" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="F101">
-        <v>238129</v>
+        <v>225104</v>
       </c>
       <c r="G101">
-        <v>2309393</v>
+        <v>2306256</v>
       </c>
       <c r="I101" t="s">
-        <v>420</v>
-      </c>
-      <c r="K101" t="s">
-        <v>589</v>
+        <v>241</v>
       </c>
       <c r="M101" s="4" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
     </row>
     <row r="102" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E102" t="s">
-        <v>423</v>
+        <v>428</v>
       </c>
       <c r="F102">
-        <v>225104</v>
+        <v>227388</v>
       </c>
       <c r="G102">
-        <v>2306256</v>
+        <v>2239468</v>
       </c>
       <c r="I102" t="s">
-        <v>241</v>
+        <v>258</v>
       </c>
       <c r="M102" s="4" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
     </row>
     <row r="103" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E103" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="F103">
-        <v>227388</v>
+        <v>231549</v>
       </c>
       <c r="G103">
-        <v>2239468</v>
-      </c>
-      <c r="I103" t="s">
-        <v>258</v>
+        <v>2269746</v>
       </c>
       <c r="M103" s="4" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
     </row>
     <row r="104" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E104" t="s">
-        <v>430</v>
+        <v>436</v>
       </c>
       <c r="F104">
-        <v>231549</v>
+        <v>297038</v>
       </c>
       <c r="G104">
-        <v>2269746</v>
+        <v>6860791</v>
+      </c>
+      <c r="H104" t="s">
+        <v>250</v>
       </c>
       <c r="M104" s="4" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
     </row>
     <row r="105" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E105" t="s">
-        <v>436</v>
+        <v>444</v>
       </c>
       <c r="F105">
-        <v>297038</v>
+        <v>76612</v>
       </c>
       <c r="G105">
-        <v>6860791</v>
-      </c>
-      <c r="H105" t="s">
-        <v>250</v>
+        <v>2242855</v>
+      </c>
+      <c r="I105" t="s">
+        <v>257</v>
       </c>
       <c r="M105" s="4" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
     </row>
     <row r="106" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E106" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
       <c r="F106">
-        <v>76612</v>
+        <v>223428</v>
       </c>
       <c r="G106">
-        <v>2242855</v>
+        <v>2260928</v>
       </c>
       <c r="I106" t="s">
-        <v>257</v>
+        <v>449</v>
       </c>
       <c r="M106" s="4" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
     </row>
     <row r="107" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E107" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="F107">
-        <v>223428</v>
+        <v>373450</v>
       </c>
       <c r="G107">
-        <v>2260928</v>
+        <v>6651814</v>
       </c>
       <c r="I107" t="s">
-        <v>449</v>
+        <v>256</v>
       </c>
       <c r="M107" s="4" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
     </row>
     <row r="108" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E108" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="F108">
-        <v>373450</v>
+        <v>224613</v>
       </c>
       <c r="G108">
-        <v>6651814</v>
+        <v>2248029</v>
       </c>
       <c r="I108" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
       <c r="M108" s="4" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
     </row>
     <row r="109" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E109" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="F109">
-        <v>224613</v>
+        <v>225921</v>
       </c>
       <c r="G109">
-        <v>2248029</v>
+        <v>2242378</v>
       </c>
       <c r="I109" t="s">
-        <v>241</v>
+        <v>255</v>
       </c>
       <c r="M109" s="4" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
     </row>
     <row r="110" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E110" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="F110">
-        <v>225921</v>
+        <v>236564</v>
       </c>
       <c r="G110">
-        <v>2242378</v>
+        <v>2346187</v>
       </c>
       <c r="I110" t="s">
-        <v>255</v>
+        <v>257</v>
+      </c>
+      <c r="K110" t="s">
+        <v>454</v>
       </c>
       <c r="M110" s="4" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
     </row>
     <row r="111" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E111" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
       <c r="F111">
-        <v>236564</v>
+        <v>241291</v>
       </c>
       <c r="G111">
-        <v>2346187</v>
+        <v>3214411</v>
       </c>
       <c r="I111" t="s">
-        <v>257</v>
-      </c>
-      <c r="K111" t="s">
-        <v>454</v>
+        <v>254</v>
       </c>
       <c r="M111" s="4" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
     </row>
     <row r="112" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E112" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="F112">
-        <v>241291</v>
+        <v>72728</v>
       </c>
       <c r="G112">
-        <v>3214411</v>
-      </c>
-      <c r="I112" t="s">
-        <v>254</v>
+        <v>2299292</v>
       </c>
       <c r="M112" s="4" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
     </row>
     <row r="113" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E113" t="s">
-        <v>458</v>
+        <v>465</v>
       </c>
       <c r="F113">
-        <v>72728</v>
+        <v>224190</v>
       </c>
       <c r="G113">
-        <v>2299292</v>
+        <v>2252223</v>
+      </c>
+      <c r="I113" t="s">
+        <v>241</v>
       </c>
       <c r="M113" s="4" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
     </row>
     <row r="114" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E114" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="F114">
-        <v>224190</v>
+        <v>564236</v>
       </c>
       <c r="G114">
-        <v>2252223</v>
+        <v>4501439</v>
       </c>
       <c r="I114" t="s">
-        <v>241</v>
+        <v>257</v>
       </c>
       <c r="M114" s="4" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
     </row>
     <row r="115" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E115" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="F115">
-        <v>564236</v>
+        <v>230867</v>
       </c>
       <c r="G115">
-        <v>4501439</v>
-      </c>
-      <c r="I115" t="s">
-        <v>257</v>
+        <v>3034568</v>
       </c>
       <c r="M115" s="4" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
     </row>
     <row r="116" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E116" t="s">
-        <v>468</v>
+        <v>489</v>
       </c>
       <c r="F116">
-        <v>230867</v>
+        <v>235442</v>
       </c>
       <c r="G116">
-        <v>3034568</v>
+        <v>2666986</v>
+      </c>
+      <c r="I116" t="s">
+        <v>259</v>
       </c>
       <c r="M116" s="4" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
     </row>
     <row r="117" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E117" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="F117">
-        <v>235442</v>
+        <v>68023</v>
       </c>
       <c r="G117">
-        <v>2666986</v>
-      </c>
-      <c r="I117" t="s">
-        <v>259</v>
+        <v>2323944</v>
       </c>
       <c r="M117" s="4" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
     </row>
     <row r="118" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E118" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="F118">
-        <v>68023</v>
+        <v>223904</v>
       </c>
       <c r="G118">
-        <v>2323944</v>
+        <v>2252359</v>
       </c>
       <c r="M118" s="4" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
     </row>
     <row r="119" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E119" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="F119">
-        <v>223904</v>
+        <v>244940</v>
       </c>
       <c r="G119">
-        <v>2252359</v>
+        <v>2328202</v>
+      </c>
+      <c r="I119" t="s">
+        <v>241</v>
       </c>
       <c r="M119" s="4" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
     </row>
     <row r="120" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E120" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="F120">
-        <v>244940</v>
+        <v>245889</v>
       </c>
       <c r="G120">
-        <v>2328202</v>
+        <v>2305675</v>
       </c>
       <c r="I120" t="s">
         <v>241</v>
       </c>
       <c r="M120" s="4" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="121" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E121" t="s">
-        <v>494</v>
+        <v>485</v>
       </c>
       <c r="F121">
-        <v>245889</v>
+        <v>237422</v>
       </c>
       <c r="G121">
-        <v>2305675</v>
+        <v>2286706</v>
       </c>
       <c r="I121" t="s">
-        <v>241</v>
+        <v>257</v>
       </c>
       <c r="M121" s="4" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
     </row>
     <row r="122" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E122" t="s">
-        <v>485</v>
+        <v>495</v>
       </c>
       <c r="F122">
-        <v>237422</v>
+        <v>238546</v>
       </c>
       <c r="G122">
-        <v>2286706</v>
+        <v>2694970</v>
       </c>
       <c r="I122" t="s">
-        <v>257</v>
+        <v>241</v>
       </c>
       <c r="M122" s="4" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
     </row>
     <row r="123" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E123" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="F123">
-        <v>238546</v>
+        <v>322896</v>
       </c>
       <c r="G123">
-        <v>2694970</v>
+        <v>3187837</v>
       </c>
       <c r="I123" t="s">
-        <v>241</v>
+        <v>254</v>
       </c>
       <c r="M123" s="4" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
     </row>
     <row r="124" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E124" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="F124">
-        <v>322896</v>
+        <v>242292</v>
       </c>
       <c r="G124">
-        <v>3187837</v>
+        <v>2373416</v>
       </c>
       <c r="I124" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="M124" s="4" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
     </row>
     <row r="125" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E125" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="F125">
-        <v>242292</v>
+        <v>261990</v>
       </c>
       <c r="G125">
-        <v>2373416</v>
+        <v>2515259</v>
       </c>
       <c r="I125" t="s">
-        <v>241</v>
+        <v>257</v>
       </c>
       <c r="M125" s="4" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
     </row>
     <row r="126" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E126" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="F126">
-        <v>261990</v>
+        <v>266184</v>
       </c>
       <c r="G126">
-        <v>2515259</v>
+        <v>2412332</v>
       </c>
       <c r="I126" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="M126" s="4" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
     </row>
     <row r="127" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E127" t="s">
-        <v>499</v>
+        <v>263</v>
       </c>
       <c r="F127">
-        <v>266184</v>
+        <v>256087</v>
       </c>
       <c r="G127">
-        <v>2412332</v>
+        <v>2444459</v>
+      </c>
+      <c r="H127" t="s">
+        <v>250</v>
       </c>
       <c r="I127" t="s">
         <v>254</v>
       </c>
       <c r="M127" s="4" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
     </row>
     <row r="128" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E128" t="s">
-        <v>263</v>
+        <v>505</v>
       </c>
       <c r="F128">
-        <v>256087</v>
+        <v>316867</v>
       </c>
       <c r="G128">
-        <v>2444459</v>
-      </c>
-      <c r="H128" t="s">
-        <v>250</v>
+        <v>3187833</v>
       </c>
       <c r="I128" t="s">
         <v>254</v>
       </c>
       <c r="M128" s="4" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
     </row>
     <row r="129" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E129" t="s">
-        <v>505</v>
+        <v>510</v>
       </c>
       <c r="F129">
-        <v>316867</v>
+        <v>55438</v>
       </c>
       <c r="G129">
-        <v>3187833</v>
+        <v>2221679</v>
       </c>
       <c r="I129" t="s">
-        <v>254</v>
+        <v>277</v>
       </c>
       <c r="M129" s="4" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
     </row>
     <row r="130" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E130" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="F130">
-        <v>55438</v>
+        <v>223548</v>
       </c>
       <c r="G130">
-        <v>2221679</v>
+        <v>2250666</v>
       </c>
       <c r="I130" t="s">
         <v>277</v>
       </c>
       <c r="M130" s="4" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
     </row>
     <row r="131" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E131" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="F131">
-        <v>223548</v>
+        <v>238003</v>
       </c>
       <c r="G131">
-        <v>2250666</v>
+        <v>2286894</v>
+      </c>
+      <c r="H131" t="s">
+        <v>250</v>
       </c>
       <c r="I131" t="s">
-        <v>277</v>
+        <v>257</v>
       </c>
       <c r="M131" s="4" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
     </row>
     <row r="132" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E132" t="s">
-        <v>513</v>
+        <v>519</v>
       </c>
       <c r="F132">
-        <v>238003</v>
+        <v>227914</v>
       </c>
       <c r="G132">
-        <v>2286894</v>
-      </c>
-      <c r="H132" t="s">
-        <v>250</v>
+        <v>6785715</v>
       </c>
       <c r="I132" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="M132" s="4" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
     </row>
     <row r="133" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E133" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="F133">
-        <v>227914</v>
+        <v>232564</v>
       </c>
       <c r="G133">
-        <v>6785715</v>
+        <v>2417787</v>
       </c>
       <c r="I133" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
       <c r="M133" s="4" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
     </row>
     <row r="134" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E134" t="s">
-        <v>520</v>
+        <v>526</v>
       </c>
       <c r="F134">
-        <v>232564</v>
+        <v>246473</v>
       </c>
       <c r="G134">
-        <v>2417787</v>
+        <v>2309489</v>
       </c>
       <c r="I134" t="s">
-        <v>241</v>
+        <v>527</v>
       </c>
       <c r="M134" s="4" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
     </row>
     <row r="135" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E135" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="F135">
-        <v>246473</v>
+        <v>227661</v>
       </c>
       <c r="G135">
-        <v>2309489</v>
+        <v>2273687</v>
       </c>
       <c r="I135" t="s">
-        <v>527</v>
+        <v>254</v>
       </c>
       <c r="M135" s="4" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
     </row>
     <row r="136" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E136" t="s">
-        <v>528</v>
+        <v>535</v>
       </c>
       <c r="F136">
-        <v>227661</v>
+        <v>229503</v>
       </c>
       <c r="G136">
-        <v>2273687</v>
+        <v>2283060</v>
       </c>
       <c r="I136" t="s">
-        <v>254</v>
+        <v>277</v>
       </c>
       <c r="M136" s="4" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
     </row>
     <row r="137" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E137" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="F137">
-        <v>229503</v>
+        <v>237533</v>
       </c>
       <c r="G137">
-        <v>2283060</v>
+        <v>2293397</v>
       </c>
       <c r="I137" t="s">
-        <v>277</v>
+        <v>241</v>
       </c>
       <c r="M137" s="4" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
     </row>
     <row r="138" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E138" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="F138">
-        <v>237533</v>
+        <v>245169</v>
       </c>
       <c r="G138">
-        <v>2293397</v>
+        <v>5083289</v>
       </c>
       <c r="I138" t="s">
         <v>241</v>
       </c>
       <c r="M138" s="4" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
     </row>
     <row r="139" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E139" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="F139">
-        <v>245169</v>
+        <v>229318</v>
       </c>
       <c r="G139">
-        <v>5083289</v>
+        <v>2300180</v>
       </c>
       <c r="I139" t="s">
         <v>241</v>
       </c>
       <c r="M139" s="4" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
     </row>
     <row r="140" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E140" t="s">
-        <v>538</v>
+        <v>541</v>
       </c>
       <c r="F140">
-        <v>229318</v>
+        <v>238803</v>
       </c>
       <c r="G140">
-        <v>2300180</v>
+        <v>2922539</v>
       </c>
       <c r="I140" t="s">
-        <v>241</v>
+        <v>255</v>
       </c>
       <c r="M140" s="4" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
     </row>
     <row r="141" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E141" t="s">
-        <v>541</v>
+        <v>546</v>
       </c>
       <c r="F141">
-        <v>238803</v>
+        <v>238353</v>
       </c>
       <c r="G141">
-        <v>2922539</v>
-      </c>
-      <c r="I141" t="s">
-        <v>255</v>
+        <v>2310104</v>
       </c>
       <c r="M141" s="4" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
     </row>
     <row r="142" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E142" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="F142">
-        <v>238353</v>
+        <v>377164</v>
       </c>
       <c r="G142">
-        <v>2310104</v>
+        <v>6924416</v>
       </c>
       <c r="M142" s="4" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
     </row>
     <row r="143" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E143" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="F143">
-        <v>377164</v>
+        <v>278475</v>
       </c>
       <c r="G143">
-        <v>6924416</v>
+        <v>2482398</v>
+      </c>
+      <c r="I143" t="s">
+        <v>550</v>
       </c>
       <c r="M143" s="4" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
     </row>
     <row r="144" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E144" t="s">
-        <v>549</v>
+        <v>558</v>
       </c>
       <c r="F144">
-        <v>278475</v>
+        <v>318646</v>
       </c>
       <c r="G144">
-        <v>2482398</v>
+        <v>3253257</v>
       </c>
       <c r="I144" t="s">
-        <v>550</v>
+        <v>254</v>
       </c>
       <c r="M144" s="4" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
     </row>
     <row r="145" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E145" t="s">
-        <v>558</v>
+        <v>567</v>
       </c>
       <c r="F145">
-        <v>318646</v>
+        <v>244959</v>
       </c>
       <c r="G145">
-        <v>3253257</v>
+        <v>2299831</v>
+      </c>
+      <c r="H145" t="s">
+        <v>250</v>
       </c>
       <c r="I145" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="M145" s="4" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
     </row>
     <row r="146" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E146" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="F146">
-        <v>244959</v>
+        <v>288957</v>
       </c>
       <c r="G146">
-        <v>2299831</v>
+        <v>5016113</v>
       </c>
       <c r="H146" t="s">
         <v>250</v>
       </c>
       <c r="I146" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
       <c r="M146" s="4" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
     </row>
     <row r="147" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E147" t="s">
-        <v>568</v>
+        <v>574</v>
       </c>
       <c r="F147">
-        <v>288957</v>
+        <v>443761</v>
       </c>
       <c r="G147">
-        <v>5016113</v>
-      </c>
-      <c r="H147" t="s">
-        <v>250</v>
+        <v>3194519</v>
       </c>
       <c r="I147" t="s">
         <v>241</v>
       </c>
       <c r="M147" s="4" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
     </row>
     <row r="148" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E148" t="s">
-        <v>574</v>
+        <v>580</v>
       </c>
       <c r="F148">
-        <v>443761</v>
+        <v>221214</v>
       </c>
       <c r="G148">
-        <v>3194519</v>
+        <v>2475630</v>
       </c>
       <c r="I148" t="s">
-        <v>241</v>
+        <v>581</v>
       </c>
       <c r="M148" s="4" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
     </row>
     <row r="149" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E149" t="s">
-        <v>580</v>
+        <v>584</v>
       </c>
       <c r="F149">
-        <v>221214</v>
+        <v>1151126</v>
       </c>
       <c r="G149">
-        <v>2475630</v>
+        <v>6933033</v>
       </c>
       <c r="I149" t="s">
-        <v>581</v>
+        <v>241</v>
       </c>
       <c r="M149" s="4" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
     </row>
     <row r="150" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E150" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="F150">
-        <v>1151126</v>
+        <v>605192</v>
       </c>
       <c r="G150">
-        <v>6933033</v>
+        <v>3777792</v>
       </c>
       <c r="I150" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="M150" s="4" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
     </row>
     <row r="151" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E151" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="F151">
-        <v>605192</v>
+        <v>237211</v>
       </c>
       <c r="G151">
-        <v>3777792</v>
+        <v>2273698</v>
       </c>
       <c r="I151" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="M151" s="4" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
     </row>
     <row r="152" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E152" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="F152">
-        <v>237211</v>
+        <v>236609</v>
       </c>
       <c r="G152">
-        <v>2273698</v>
+        <v>2941926</v>
       </c>
       <c r="I152" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="M152" s="4" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
     </row>
     <row r="153" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E153" t="s">
-        <v>587</v>
+        <v>502</v>
       </c>
       <c r="F153">
-        <v>236609</v>
+        <v>59769</v>
       </c>
       <c r="G153">
-        <v>2941926</v>
+        <v>2210527</v>
       </c>
       <c r="I153" t="s">
+        <v>503</v>
+      </c>
+      <c r="L153" t="s">
+        <v>628</v>
+      </c>
+      <c r="M153" s="4" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="154" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="E154" s="9" t="s">
+        <v>346</v>
+      </c>
+      <c r="F154" s="9">
+        <v>243712</v>
+      </c>
+      <c r="G154" s="9">
+        <v>2299739</v>
+      </c>
+      <c r="H154" s="9"/>
+      <c r="I154" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="M153" s="4" t="s">
-        <v>843</v>
-      </c>
-    </row>
-    <row r="154" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E154" t="s">
-        <v>502</v>
-      </c>
-      <c r="F154">
-        <v>59769</v>
-      </c>
-      <c r="G154">
-        <v>2210527</v>
-      </c>
-      <c r="I154" t="s">
-        <v>503</v>
-      </c>
-      <c r="L154" t="s">
-        <v>628</v>
-      </c>
+      <c r="J154" s="9"/>
+      <c r="K154" s="9"/>
+      <c r="L154" s="9"/>
       <c r="M154" s="4" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
     </row>
     <row r="155" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E155" s="9" t="s">
-        <v>346</v>
-      </c>
-      <c r="F155" s="9">
-        <v>243712</v>
-      </c>
-      <c r="G155" s="9">
-        <v>2299739</v>
-      </c>
-      <c r="H155" s="9"/>
-      <c r="I155" s="9" t="s">
-        <v>241</v>
-      </c>
-      <c r="J155" s="9"/>
-      <c r="K155" s="9"/>
-      <c r="L155" s="9"/>
-      <c r="M155" s="4" t="s">
-        <v>845</v>
+      <c r="E155" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="F155" s="19">
+        <v>1031274</v>
+      </c>
+      <c r="G155" s="19">
+        <v>6039947</v>
+      </c>
+      <c r="H155" s="19"/>
+      <c r="I155" s="19" t="s">
+        <v>255</v>
+      </c>
+      <c r="J155" s="19"/>
+      <c r="K155" s="19"/>
+      <c r="L155" s="19" t="s">
+        <v>600</v>
+      </c>
+      <c r="M155" s="17" t="s">
+        <v>735</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I1:J98 I156:J1048576">
-    <cfRule type="cellIs" dxfId="19" priority="7" operator="equal">
+  <conditionalFormatting sqref="I1:J97 I156:J1048576">
+    <cfRule type="cellIs" dxfId="31" priority="9" operator="equal">
       <formula>"Custom License"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="10" operator="equal">
       <formula>"All Rights Reserved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I101:J155">
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
+  <conditionalFormatting sqref="I100:J154">
+    <cfRule type="cellIs" dxfId="29" priority="3" operator="equal">
       <formula>"Custom License"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="4" operator="equal">
+      <formula>"All Rights Reserved"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I155:J155">
+    <cfRule type="cellIs" dxfId="27" priority="1" operator="equal">
+      <formula>"Custom License"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="2" operator="equal">
       <formula>"All Rights Reserved"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="M153" r:id="rId1" xr:uid="{0297EA0E-AABC-42E6-BD9C-C92D40E3D114}"/>
+    <hyperlink ref="M152" r:id="rId1" xr:uid="{0297EA0E-AABC-42E6-BD9C-C92D40E3D114}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -6585,25 +6710,25 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="9" t="s">
         <v>576</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>577</v>
       </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18" t="s">
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9" t="s">
         <v>875</v>
       </c>
-      <c r="H7" s="18"/>
+      <c r="H7" s="9"/>
       <c r="I7" s="10" t="str">
         <f>LEFT(B7, FIND("/releases", B7) - 1)</f>
         <v>https://github.com/GTNewHorizons/Nuclear-Control</v>
       </c>
-      <c r="J7" s="18" t="str">
+      <c r="J7" s="9" t="str">
         <f>IF(D7&lt;&gt;"", D7, RIGHT(B7,LEN(B7)-FIND("@",SUBSTITUTE(B7,"/","@",LEN(B7)-LEN(SUBSTITUTE(B7,"/",""))))))</f>
         <v>IC2NuclearControl-2.6.19.jar</v>
       </c>
@@ -6622,12 +6747,12 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:O119"/>
+  <dimension ref="A1:O120"/>
   <sheetViews>
     <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="E115" sqref="E115"/>
+      <selection pane="bottomLeft" activeCell="J122" sqref="J122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -8324,7 +8449,7 @@
         <v>480</v>
       </c>
       <c r="M94" s="4" t="e">
-        <f>LEFT(F94, FIND("/releases", F94) - 1)</f>
+        <f t="shared" ref="M94:M120" si="6">LEFT(F94, FIND("/releases", F94) - 1)</f>
         <v>#VALUE!</v>
       </c>
       <c r="N94" t="str">
@@ -8343,7 +8468,7 @@
         <v>250</v>
       </c>
       <c r="M95" s="4" t="e">
-        <f>LEFT(F95, FIND("/releases", F95) - 1)</f>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="N95" t="str">
@@ -8362,7 +8487,7 @@
         <v>488</v>
       </c>
       <c r="M96" s="4" t="str">
-        <f>LEFT(F96, FIND("/releases", F96) - 1)</f>
+        <f t="shared" si="6"/>
         <v>https://github.com/GTNewHorizons/LogisticsPipes</v>
       </c>
       <c r="N96" t="str">
@@ -8378,7 +8503,7 @@
         <v>508</v>
       </c>
       <c r="M97" s="4" t="e">
-        <f>LEFT(F97, FIND("/releases", F97) - 1)</f>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="N97" t="str">
@@ -8394,11 +8519,11 @@
         <v>210</v>
       </c>
       <c r="M98" s="4" t="e">
-        <f>LEFT(F98, FIND("/releases", F98) - 1)</f>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="N98" t="str">
-        <f>IF(H98&lt;&gt;"", H98, RIGHT(F98,LEN(F98)-FIND("@",SUBSTITUTE(F98,"/","@",LEN(F98)-LEN(SUBSTITUTE(F98,"/",""))))))</f>
+        <f t="shared" ref="N98:N119" si="7">IF(H98&lt;&gt;"", H98, RIGHT(F98,LEN(F98)-FIND("@",SUBSTITUTE(F98,"/","@",LEN(F98)-LEN(SUBSTITUTE(F98,"/",""))))))</f>
         <v>SolarExpansion-Basic-1.6a.jar</v>
       </c>
     </row>
@@ -8413,11 +8538,11 @@
         <v>277</v>
       </c>
       <c r="M99" s="4" t="str">
-        <f>LEFT(F99, FIND("/releases", F99) - 1)</f>
+        <f t="shared" si="6"/>
         <v>https://github.com/GTNewHorizons/ThaumicEnergistics</v>
       </c>
       <c r="N99" t="str">
-        <f>IF(H99&lt;&gt;"", H99, RIGHT(F99,LEN(F99)-FIND("@",SUBSTITUTE(F99,"/","@",LEN(F99)-LEN(SUBSTITUTE(F99,"/",""))))))</f>
+        <f t="shared" si="7"/>
         <v>thaumicenergistics-1.7.11-GTNH.jar</v>
       </c>
     </row>
@@ -8432,11 +8557,11 @@
         <v>516</v>
       </c>
       <c r="M100" s="4" t="str">
-        <f>LEFT(F100, FIND("/releases", F100) - 1)</f>
+        <f t="shared" si="6"/>
         <v>https://github.com/GTNewHorizons/Thaumic_Exploration</v>
       </c>
       <c r="N100" t="str">
-        <f>IF(H100&lt;&gt;"", H100, RIGHT(F100,LEN(F100)-FIND("@",SUBSTITUTE(F100,"/","@",LEN(F100)-LEN(SUBSTITUTE(F100,"/",""))))))</f>
+        <f t="shared" si="7"/>
         <v>Thaumic-Exploration-1.4.6-GTNH-pre.jar</v>
       </c>
     </row>
@@ -8451,11 +8576,11 @@
         <v>523</v>
       </c>
       <c r="M101" s="4" t="str">
-        <f>LEFT(F101, FIND("/releases", F101) - 1)</f>
+        <f t="shared" si="6"/>
         <v>https://github.com/GTNewHorizons/ThaumicTinkerer</v>
       </c>
       <c r="N101" t="str">
-        <f>IF(H101&lt;&gt;"", H101, RIGHT(F101,LEN(F101)-FIND("@",SUBSTITUTE(F101,"/","@",LEN(F101)-LEN(SUBSTITUTE(F101,"/",""))))))</f>
+        <f t="shared" si="7"/>
         <v>ThaumicTinkerer-2.11.20.jar</v>
       </c>
     </row>
@@ -8470,11 +8595,11 @@
         <v>426</v>
       </c>
       <c r="M102" s="4" t="str">
-        <f>LEFT(F102, FIND("/releases", F102) - 1)</f>
+        <f t="shared" si="6"/>
         <v>https://github.com/GTNewHorizons/twilightforest</v>
       </c>
       <c r="N102" t="str">
-        <f>IF(H102&lt;&gt;"", H102, RIGHT(F102,LEN(F102)-FIND("@",SUBSTITUTE(F102,"/","@",LEN(F102)-LEN(SUBSTITUTE(F102,"/",""))))))</f>
+        <f t="shared" si="7"/>
         <v>TwilightForest-2.7.11.jar</v>
       </c>
     </row>
@@ -8492,11 +8617,11 @@
         <v>531</v>
       </c>
       <c r="M103" s="4" t="str">
-        <f>LEFT(F103, FIND("/releases", F103) - 1)</f>
+        <f t="shared" si="6"/>
         <v>https://github.com/GTNewHorizons/TiC-Tooltips</v>
       </c>
       <c r="N103" t="str">
-        <f>IF(H103&lt;&gt;"", H103, RIGHT(F103,LEN(F103)-FIND("@",SUBSTITUTE(F103,"/","@",LEN(F103)-LEN(SUBSTITUTE(F103,"/",""))))))</f>
+        <f t="shared" si="7"/>
         <v>TiCTooltips-1.4.0.jar</v>
       </c>
     </row>
@@ -8511,11 +8636,11 @@
         <v>283</v>
       </c>
       <c r="M104" s="4" t="str">
-        <f>LEFT(F104, FIND("/releases", F104) - 1)</f>
+        <f t="shared" si="6"/>
         <v>https://github.com/GTNewHorizons/TinkersMechworks</v>
       </c>
       <c r="N104" t="str">
-        <f>IF(H104&lt;&gt;"", H104, RIGHT(F104,LEN(F104)-FIND("@",SUBSTITUTE(F104,"/","@",LEN(F104)-LEN(SUBSTITUTE(F104,"/",""))))))</f>
+        <f t="shared" si="7"/>
         <v>TMechworks-0.4.1.jar</v>
       </c>
     </row>
@@ -8527,11 +8652,11 @@
         <v>540</v>
       </c>
       <c r="M105" s="4" t="e">
-        <f>LEFT(F105, FIND("/releases", F105) - 1)</f>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="N105" t="str">
-        <f>IF(H105&lt;&gt;"", H105, RIGHT(F105,LEN(F105)-FIND("@",SUBSTITUTE(F105,"/","@",LEN(F105)-LEN(SUBSTITUTE(F105,"/",""))))))</f>
+        <f t="shared" si="7"/>
         <v>tubestuff-59.0.4.jar</v>
       </c>
     </row>
@@ -8543,11 +8668,11 @@
         <v>544</v>
       </c>
       <c r="M106" s="4" t="e">
-        <f>LEFT(F106, FIND("/releases", F106) - 1)</f>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="N106" t="str">
-        <f>IF(H106&lt;&gt;"", H106, RIGHT(F106,LEN(F106)-FIND("@",SUBSTITUTE(F106,"/","@",LEN(F106)-LEN(SUBSTITUTE(F106,"/",""))))))</f>
+        <f t="shared" si="7"/>
         <v>UniverseCraft-1.7.10-V1.4.2.jar</v>
       </c>
     </row>
@@ -8559,11 +8684,11 @@
         <v>553</v>
       </c>
       <c r="M107" s="4" t="str">
-        <f>LEFT(F107, FIND("/releases", F107) - 1)</f>
+        <f t="shared" si="6"/>
         <v>https://github.com/GTNewHorizons/gendustry</v>
       </c>
       <c r="N107" t="str">
-        <f>IF(H107&lt;&gt;"", H107, RIGHT(F107,LEN(F107)-FIND("@",SUBSTITUTE(F107,"/","@",LEN(F107)-LEN(SUBSTITUTE(F107,"/",""))))))</f>
+        <f t="shared" si="7"/>
         <v>gendustry-1.9.4-GTNH.jar</v>
       </c>
     </row>
@@ -8575,11 +8700,11 @@
         <v>559</v>
       </c>
       <c r="M108" s="4" t="str">
-        <f>LEFT(F108, FIND("/releases", F108) - 1)</f>
+        <f t="shared" si="6"/>
         <v>https://github.com/Jonius7/EnderIOAddons</v>
       </c>
       <c r="N108" t="str">
-        <f>IF(H108&lt;&gt;"", H108, RIGHT(F108,LEN(F108)-FIND("@",SUBSTITUTE(F108,"/","@",LEN(F108)-LEN(SUBSTITUTE(F108,"/",""))))))</f>
+        <f t="shared" si="7"/>
         <v>enderioaddons-1.7.10-0.10.16.jar</v>
       </c>
     </row>
@@ -8597,11 +8722,11 @@
         <v>563</v>
       </c>
       <c r="M109" s="4" t="str">
-        <f>LEFT(F109, FIND("/releases", F109) - 1)</f>
+        <f t="shared" si="6"/>
         <v>https://github.com/GTNewHorizons/AkashicTome</v>
       </c>
       <c r="N109" t="str">
-        <f>IF(H109&lt;&gt;"", H109, RIGHT(F109,LEN(F109)-FIND("@",SUBSTITUTE(F109,"/","@",LEN(F109)-LEN(SUBSTITUTE(F109,"/",""))))))</f>
+        <f t="shared" si="7"/>
         <v>akashictome-1.2.6.jar</v>
       </c>
     </row>
@@ -8619,11 +8744,11 @@
         <v>283</v>
       </c>
       <c r="M110" s="4" t="str">
-        <f>LEFT(F110, FIND("/releases", F110) - 1)</f>
+        <f t="shared" si="6"/>
         <v>https://github.com/idkidknow/IE1710NEIPatch</v>
       </c>
       <c r="N110" t="str">
-        <f>IF(H110&lt;&gt;"", H110, RIGHT(F110,LEN(F110)-FIND("@",SUBSTITUTE(F110,"/","@",LEN(F110)-LEN(SUBSTITUTE(F110,"/",""))))))</f>
+        <f t="shared" si="7"/>
         <v>ie1710neipatch-0.1.1.jar</v>
       </c>
     </row>
@@ -8635,11 +8760,11 @@
         <v>572</v>
       </c>
       <c r="M111" s="4" t="str">
-        <f>LEFT(F111, FIND("/releases", F111) - 1)</f>
+        <f t="shared" si="6"/>
         <v>https://github.com/GTNewHorizons/FTB-Utilities</v>
       </c>
       <c r="N111" t="str">
-        <f>IF(H111&lt;&gt;"", H111, RIGHT(F111,LEN(F111)-FIND("@",SUBSTITUTE(F111,"/","@",LEN(F111)-LEN(SUBSTITUTE(F111,"/",""))))))</f>
+        <f t="shared" si="7"/>
         <v>FTBUtilities-1.1.1-GTNH.jar</v>
       </c>
     </row>
@@ -8654,11 +8779,11 @@
         <v>254</v>
       </c>
       <c r="M112" s="4" t="str">
-        <f>LEFT(F112, FIND("/releases", F112) - 1)</f>
+        <f t="shared" si="6"/>
         <v>https://github.com/GTNewHorizons/ProjectBlue</v>
       </c>
       <c r="N112" t="str">
-        <f>IF(H112&lt;&gt;"", H112, RIGHT(F112,LEN(F112)-FIND("@",SUBSTITUTE(F112,"/","@",LEN(F112)-LEN(SUBSTITUTE(F112,"/",""))))))</f>
+        <f t="shared" si="7"/>
         <v>ProjectBlue-1.2.0-GTNH.jar</v>
       </c>
     </row>
@@ -8673,11 +8798,11 @@
         <v>283</v>
       </c>
       <c r="M113" s="4" t="str">
-        <f>LEFT(F113, FIND("/releases", F113) - 1)</f>
+        <f t="shared" si="6"/>
         <v>https://github.com/GTNewHorizons/WirelessRedstone-CBE</v>
       </c>
       <c r="N113" t="str">
-        <f>IF(H113&lt;&gt;"", H113, RIGHT(F113,LEN(F113)-FIND("@",SUBSTITUTE(F113,"/","@",LEN(F113)-LEN(SUBSTITUTE(F113,"/",""))))))</f>
+        <f t="shared" si="7"/>
         <v>WR-CBE-1.7.1.jar</v>
       </c>
     </row>
@@ -8692,11 +8817,11 @@
         <v>297</v>
       </c>
       <c r="M114" s="4" t="str">
-        <f>LEFT(F114, FIND("/releases", F114) - 1)</f>
+        <f t="shared" si="6"/>
         <v>https://github.com/GTNewHorizons/Chisel</v>
       </c>
       <c r="N114" t="str">
-        <f>IF(H114&lt;&gt;"", H114, RIGHT(F114,LEN(F114)-FIND("@",SUBSTITUTE(F114,"/","@",LEN(F114)-LEN(SUBSTITUTE(F114,"/",""))))))</f>
+        <f t="shared" si="7"/>
         <v>chisel-2.16.11-GTNH.jar</v>
       </c>
     </row>
@@ -8711,11 +8836,11 @@
         <v>591</v>
       </c>
       <c r="M115" s="4" t="str">
-        <f>LEFT(F115, FIND("/releases", F115) - 1)</f>
+        <f t="shared" si="6"/>
         <v>https://github.com/DrParadox7/Binnie</v>
       </c>
       <c r="N115" t="str">
-        <f>IF(H115&lt;&gt;"", H115, RIGHT(F115,LEN(F115)-FIND("@",SUBSTITUTE(F115,"/","@",LEN(F115)-LEN(SUBSTITUTE(F115,"/",""))))))</f>
+        <f t="shared" si="7"/>
         <v>binnie-mods-v2.1.15-LE.jar</v>
       </c>
     </row>
@@ -8730,11 +8855,11 @@
         <v>283</v>
       </c>
       <c r="M116" s="4" t="str">
-        <f>LEFT(F116, FIND("/releases", F116) - 1)</f>
+        <f t="shared" si="6"/>
         <v>https://github.com/Jonius7/NuclearCraft</v>
       </c>
       <c r="N116" t="str">
-        <f>IF(H116&lt;&gt;"", H116, RIGHT(F116,LEN(F116)-FIND("@",SUBSTITUTE(F116,"/","@",LEN(F116)-LEN(SUBSTITUTE(F116,"/",""))))))</f>
+        <f t="shared" si="7"/>
         <v>NuclearCraft-1.9h--1.7.10.jar</v>
       </c>
     </row>
@@ -8749,11 +8874,11 @@
         <v>283</v>
       </c>
       <c r="M117" s="4" t="str">
-        <f>LEFT(F117, FIND("/releases", F117) - 1)</f>
+        <f t="shared" si="6"/>
         <v>https://github.com/GTNewHorizons/BetterQuesting</v>
       </c>
       <c r="N117" t="str">
-        <f>IF(H117&lt;&gt;"", H117, RIGHT(F117,LEN(F117)-FIND("@",SUBSTITUTE(F117,"/","@",LEN(F117)-LEN(SUBSTITUTE(F117,"/",""))))))</f>
+        <f t="shared" si="7"/>
         <v>BetterQuesting-3.7.13-GTNH.jar</v>
       </c>
     </row>
@@ -8768,11 +8893,11 @@
         <v>686</v>
       </c>
       <c r="M118" s="4" t="e">
-        <f>LEFT(F118, FIND("/releases", F118) - 1)</f>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="N118" t="str">
-        <f>IF(H118&lt;&gt;"", H118, RIGHT(F118,LEN(F118)-FIND("@",SUBSTITUTE(F118,"/","@",LEN(F118)-LEN(SUBSTITUTE(F118,"/",""))))))</f>
+        <f t="shared" si="7"/>
         <v>ztech1.7.10-0.0.3.jar</v>
       </c>
     </row>
@@ -8784,20 +8909,39 @@
         <v>874</v>
       </c>
       <c r="M119" s="4" t="e">
-        <f>LEFT(F119, FIND("/releases", F119) - 1)</f>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="N119" t="str">
-        <f>IF(H119&lt;&gt;"", H119, RIGHT(F119,LEN(F119)-FIND("@",SUBSTITUTE(F119,"/","@",LEN(F119)-LEN(SUBSTITUTE(F119,"/",""))))))</f>
+        <f t="shared" si="7"/>
         <v>Technomancy - 0.12.5 - 1.7.10.jar</v>
+      </c>
+    </row>
+    <row r="120" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="E120" t="s">
+        <v>883</v>
+      </c>
+      <c r="F120" s="23" t="s">
+        <v>884</v>
+      </c>
+      <c r="J120" t="s">
+        <v>283</v>
+      </c>
+      <c r="M120" s="4" t="str">
+        <f t="shared" si="6"/>
+        <v>https://github.com/Myask-sl/adjachest-1.7.10</v>
+      </c>
+      <c r="N120" s="24" t="str">
+        <f>IF(H120&lt;&gt;"", H120, RIGHT(F120,LEN(F120)-FIND("@",SUBSTITUTE(F120,"/","@",LEN(F120)-LEN(SUBSTITUTE(F120,"/",""))))))</f>
+        <v>adjachest-0.9.9.9beta10.jar</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="J3">
-    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="1" operator="equal">
       <formula>"Custom License"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="2" operator="equal">
       <formula>"All Rights Reserved"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8937,7 +9081,7 @@
       <selection activeCell="E1" sqref="E1"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
-      <selection pane="bottomRight" activeCell="I29" sqref="I29"/>
+      <selection pane="bottomRight" activeCell="E29" sqref="E29:M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -9538,11 +9682,11 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
+  <conditionalFormatting sqref="I1:I28 I30:I1048576">
+    <cfRule type="cellIs" dxfId="23" priority="3" operator="equal">
       <formula>"Custom License"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="4" operator="equal">
       <formula>"All Rights Reserved"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10227,10 +10371,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E8BB584-5680-4F0E-93DA-8135C8293787}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10288,31 +10432,31 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="18" t="s">
         <v>244</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="18" t="s">
         <v>249</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="18" t="s">
         <v>239</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="18" t="s">
         <v>288</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="18" t="s">
         <v>263</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="H5" s="18" t="s">
         <v>342</v>
       </c>
-      <c r="I5" s="19" t="s">
+      <c r="I5" s="18" t="s">
         <v>692</v>
       </c>
     </row>
@@ -10500,7 +10644,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>414</v>
       </c>
@@ -10517,7 +10661,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>592</v>
       </c>
@@ -10531,7 +10675,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>165</v>
       </c>
@@ -10551,7 +10695,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>564</v>
       </c>
@@ -10568,7 +10712,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
         <v>565</v>
       </c>
@@ -10588,7 +10732,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>566</v>
       </c>
@@ -10605,7 +10749,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>181</v>
       </c>
@@ -10622,40 +10766,127 @@
         <v>588</v>
       </c>
     </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="20" t="s">
+        <v>885</v>
+      </c>
+      <c r="B24" s="20">
+        <v>1065808</v>
+      </c>
+      <c r="C24" s="20">
+        <v>7027153</v>
+      </c>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20" t="s">
+        <v>255</v>
+      </c>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="16" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="21" t="s">
+        <v>889</v>
+      </c>
+      <c r="B25" s="21">
+        <v>665627</v>
+      </c>
+      <c r="C25" s="21">
+        <v>6974712</v>
+      </c>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21" t="s">
+        <v>255</v>
+      </c>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="25" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="22" t="s">
+        <v>886</v>
+      </c>
+      <c r="B26" s="22">
+        <v>665744</v>
+      </c>
+      <c r="C26" s="22">
+        <v>7020357</v>
+      </c>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22" t="s">
+        <v>255</v>
+      </c>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="15" t="s">
+        <v>888</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="E6:E18">
-    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
       <formula>"Custom License"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="20" operator="equal">
       <formula>"All Rights Reserved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20:E22">
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="15" operator="equal">
       <formula>"Custom License"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="16" operator="equal">
+      <formula>"All Rights Reserved"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5:F5">
+    <cfRule type="cellIs" dxfId="15" priority="11" operator="equal">
+      <formula>"Custom License"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="12" operator="equal">
       <formula>"All Rights Reserved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19:F19">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="17" operator="equal">
       <formula>"Custom License"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="18" operator="equal">
       <formula>"All Rights Reserved"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23:F23">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
       <formula>"Custom License"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="14" operator="equal">
       <formula>"All Rights Reserved"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E5:F5">
+  <conditionalFormatting sqref="E26:F26">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+      <formula>"Custom License"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+      <formula>"All Rights Reserved"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"Custom License"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>"All Rights Reserved"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E24:F24">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Custom License"</formula>
     </cfRule>

</xml_diff>